<commit_message>
#feat: add rule file
</commit_message>
<xml_diff>
--- a/docs/specs/Checklist.xlsx
+++ b/docs/specs/Checklist.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Template Source\VUE\vue-mocha\docs\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09FC42A3-54D7-4C2E-AD8F-BF583B255A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0630F225-2B75-4BD0-913B-A506C9115A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover " sheetId="3" r:id="rId1"/>
-    <sheet name="Checklist" sheetId="1" r:id="rId2"/>
-    <sheet name="tsdoc" sheetId="5" r:id="rId3"/>
-    <sheet name="Code Order" sheetId="6" r:id="rId4"/>
-    <sheet name="Layout" sheetId="7" r:id="rId5"/>
+    <sheet name="Output mong muốn" sheetId="8" r:id="rId2"/>
+    <sheet name="Checklist" sheetId="1" r:id="rId3"/>
+    <sheet name="tsdoc" sheetId="5" r:id="rId4"/>
+    <sheet name="Code Order" sheetId="6" r:id="rId5"/>
+    <sheet name="Layout" sheetId="7" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="___" hidden="1">'[1]#REF'!#REF!</definedName>
@@ -190,7 +191,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="143">
   <si>
     <t>Question</t>
   </si>
@@ -612,6 +613,51 @@
   <si>
     <t>3. Check cả layout ở 1024 * 768  không được vỡ layout</t>
   </si>
+  <si>
+    <t>1. Trước khi đưa code lên</t>
+  </si>
+  <si>
+    <t>- Check hết tất cả rule trong checklist</t>
+  </si>
+  <si>
+    <t>- Chạy lint để không còn warning</t>
+  </si>
+  <si>
+    <t>2. Phần coding</t>
+  </si>
+  <si>
+    <t>- Sau khi code xong phải tối ưu lại code nếu có</t>
+  </si>
+  <si>
+    <t>- Đặt tên biến rõ ràng đúng ý nghĩa, add tsdoc rõ ràng</t>
+  </si>
+  <si>
+    <t>- Cài eslint và prettier format code</t>
+  </si>
+  <si>
+    <t>3. Phần Unit test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">- Yêu cầu coverage &gt;= 80% </t>
+  </si>
+  <si>
+    <t>- Code rõ ràng, xóa hết code thừa k sử dụng</t>
+  </si>
+  <si>
+    <t>4. Hướng dẫn</t>
+  </si>
+  <si>
+    <t>- Project sử dụng lib primevue, primeflex =&gt; Tận dụng hết tất cả component của lib trước</t>
+  </si>
+  <si>
+    <t>- Project đang viết vue3 setup script nên viết theo đúng kiểu của code mẫu đang sử dụng</t>
+  </si>
+  <si>
+    <t>- Unit test sử dụng mocha + sinon + chai =&gt; có gì thì search theo các keyword này để tìm hiểu</t>
+  </si>
+  <si>
+    <t>- Tham khảo cấu trúc thư mục hiện tại để làm theo</t>
+  </si>
 </sst>
 </file>
 
@@ -621,7 +667,7 @@
     <numFmt numFmtId="164" formatCode="yyyy/mm/dd"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -700,6 +746,14 @@
       <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -822,7 +876,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -893,15 +947,36 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -911,26 +986,38 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1333,7 +1420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:E18"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageLayout" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -2131,6 +2218,533 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14A85404-3A40-4CA2-8D80-1BD7AEC101DF}">
+  <dimension ref="A2:Z29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="39"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="41" t="s">
+        <v>128</v>
+      </c>
+      <c r="P2" s="45"/>
+      <c r="Q2" s="45"/>
+      <c r="R2" s="45"/>
+      <c r="S2" s="45"/>
+      <c r="T2" s="45"/>
+      <c r="U2" s="45"/>
+      <c r="V2" s="45"/>
+      <c r="W2" s="45"/>
+      <c r="X2" s="45"/>
+      <c r="Y2" s="45"/>
+      <c r="Z2" s="43"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B3" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="P3" s="45"/>
+      <c r="Q3" s="46"/>
+      <c r="R3" s="45"/>
+      <c r="S3" s="45"/>
+      <c r="T3" s="45"/>
+      <c r="U3" s="45"/>
+      <c r="V3" s="45"/>
+      <c r="W3" s="45"/>
+      <c r="X3" s="45"/>
+      <c r="Y3" s="45"/>
+      <c r="Z3" s="44"/>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B4" s="40" t="s">
+        <v>130</v>
+      </c>
+      <c r="P4" s="45"/>
+      <c r="Q4" s="45"/>
+      <c r="R4" s="45"/>
+      <c r="S4" s="45"/>
+      <c r="T4" s="45"/>
+      <c r="U4" s="45"/>
+      <c r="V4" s="45"/>
+      <c r="W4" s="45"/>
+      <c r="X4" s="45"/>
+      <c r="Y4" s="45"/>
+      <c r="Z4" s="44"/>
+    </row>
+    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="40" t="s">
+        <v>134</v>
+      </c>
+      <c r="P5" s="47"/>
+      <c r="Q5" s="48"/>
+      <c r="R5" s="48"/>
+      <c r="S5" s="48"/>
+      <c r="T5" s="48"/>
+      <c r="U5" s="48"/>
+      <c r="V5" s="48"/>
+      <c r="W5" s="48"/>
+      <c r="X5" s="48"/>
+      <c r="Y5" s="48"/>
+      <c r="Z5" s="44"/>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="P6" s="45"/>
+      <c r="Q6" s="45"/>
+      <c r="R6" s="45"/>
+      <c r="S6" s="45"/>
+      <c r="T6" s="45"/>
+      <c r="U6" s="45"/>
+      <c r="V6" s="45"/>
+      <c r="W6" s="45"/>
+      <c r="X6" s="45"/>
+      <c r="Y6" s="45"/>
+      <c r="Z6" s="44"/>
+    </row>
+    <row r="7" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="41" t="s">
+        <v>131</v>
+      </c>
+      <c r="P7" s="45"/>
+      <c r="Q7" s="45"/>
+      <c r="R7" s="45"/>
+      <c r="S7" s="45"/>
+      <c r="T7" s="45"/>
+      <c r="U7" s="45"/>
+      <c r="V7" s="45"/>
+      <c r="W7" s="45"/>
+      <c r="X7" s="45"/>
+      <c r="Y7" s="45"/>
+      <c r="Z7" s="43"/>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B8" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="P8" s="45"/>
+      <c r="Q8" s="45"/>
+      <c r="R8" s="45"/>
+      <c r="S8" s="45"/>
+      <c r="T8" s="45"/>
+      <c r="U8" s="45"/>
+      <c r="V8" s="45"/>
+      <c r="W8" s="45"/>
+      <c r="X8" s="45"/>
+      <c r="Y8" s="45"/>
+      <c r="Z8" s="44"/>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B9" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="P9" s="45"/>
+      <c r="Q9" s="45"/>
+      <c r="R9" s="45"/>
+      <c r="S9" s="45"/>
+      <c r="T9" s="45"/>
+      <c r="U9" s="45"/>
+      <c r="V9" s="45"/>
+      <c r="W9" s="45"/>
+      <c r="X9" s="45"/>
+      <c r="Y9" s="45"/>
+      <c r="Z9" s="44"/>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B10" s="40"/>
+      <c r="P10" s="45"/>
+      <c r="Q10" s="45"/>
+      <c r="R10" s="45"/>
+      <c r="S10" s="45"/>
+      <c r="T10" s="45"/>
+      <c r="U10" s="45"/>
+      <c r="V10" s="45"/>
+      <c r="W10" s="45"/>
+      <c r="X10" s="45"/>
+      <c r="Y10" s="45"/>
+      <c r="Z10" s="44"/>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="P11" s="45"/>
+      <c r="Q11" s="45"/>
+      <c r="R11" s="45"/>
+      <c r="S11" s="45"/>
+      <c r="T11" s="45"/>
+      <c r="U11" s="45"/>
+      <c r="V11" s="45"/>
+      <c r="W11" s="45"/>
+      <c r="X11" s="45"/>
+      <c r="Y11" s="45"/>
+      <c r="Z11" s="44"/>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="P12" s="45"/>
+      <c r="Q12" s="45"/>
+      <c r="R12" s="45"/>
+      <c r="S12" s="45"/>
+      <c r="T12" s="45"/>
+      <c r="U12" s="45"/>
+      <c r="V12" s="45"/>
+      <c r="W12" s="45"/>
+      <c r="X12" s="45"/>
+      <c r="Y12" s="45"/>
+      <c r="Z12" s="44"/>
+    </row>
+    <row r="13" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="41" t="s">
+        <v>135</v>
+      </c>
+      <c r="P13" s="45"/>
+      <c r="Q13" s="45"/>
+      <c r="R13" s="45"/>
+      <c r="S13" s="45"/>
+      <c r="T13" s="45"/>
+      <c r="U13" s="45"/>
+      <c r="V13" s="45"/>
+      <c r="W13" s="45"/>
+      <c r="X13" s="45"/>
+      <c r="Y13" s="45"/>
+      <c r="Z13" s="43"/>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B14" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="P14" s="45"/>
+      <c r="Q14" s="45"/>
+      <c r="R14" s="45"/>
+      <c r="S14" s="45"/>
+      <c r="T14" s="45"/>
+      <c r="U14" s="45"/>
+      <c r="V14" s="45"/>
+      <c r="W14" s="45"/>
+      <c r="X14" s="45"/>
+      <c r="Y14" s="45"/>
+      <c r="Z14" s="44"/>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="B15" s="40" t="s">
+        <v>137</v>
+      </c>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
+      <c r="T15" s="45"/>
+      <c r="U15" s="45"/>
+      <c r="V15" s="45"/>
+      <c r="W15" s="45"/>
+      <c r="X15" s="45"/>
+      <c r="Y15" s="45"/>
+      <c r="Z15" s="44"/>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="P16" s="45"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="45"/>
+      <c r="S16" s="45"/>
+      <c r="T16" s="45"/>
+      <c r="U16" s="45"/>
+      <c r="V16" s="45"/>
+      <c r="W16" s="45"/>
+      <c r="X16" s="45"/>
+      <c r="Y16" s="45"/>
+      <c r="Z16" s="44"/>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="P17" s="45"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="45"/>
+      <c r="S17" s="45"/>
+      <c r="T17" s="45"/>
+      <c r="U17" s="45"/>
+      <c r="V17" s="45"/>
+      <c r="W17" s="45"/>
+      <c r="X17" s="45"/>
+      <c r="Y17" s="45"/>
+      <c r="Z17" s="44"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="P18" s="45"/>
+      <c r="Q18" s="45"/>
+      <c r="R18" s="45"/>
+      <c r="S18" s="45"/>
+      <c r="T18" s="45"/>
+      <c r="U18" s="45"/>
+      <c r="V18" s="45"/>
+      <c r="W18" s="45"/>
+      <c r="X18" s="45"/>
+      <c r="Y18" s="45"/>
+      <c r="Z18" s="44"/>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="P19" s="45"/>
+      <c r="Q19" s="45"/>
+      <c r="R19" s="45"/>
+      <c r="S19" s="45"/>
+      <c r="T19" s="45"/>
+      <c r="U19" s="45"/>
+      <c r="V19" s="45"/>
+      <c r="W19" s="45"/>
+      <c r="X19" s="45"/>
+      <c r="Y19" s="45"/>
+      <c r="Z19" s="44"/>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" s="41" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="41"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="41"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="41"/>
+      <c r="P20" s="45"/>
+      <c r="Q20" s="45"/>
+      <c r="R20" s="45"/>
+      <c r="S20" s="45"/>
+      <c r="T20" s="45"/>
+      <c r="U20" s="45"/>
+      <c r="V20" s="45"/>
+      <c r="W20" s="45"/>
+      <c r="X20" s="45"/>
+      <c r="Y20" s="45"/>
+      <c r="Z20" s="44"/>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="42"/>
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42"/>
+      <c r="E21" s="42"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="42"/>
+      <c r="P21" s="45"/>
+      <c r="Q21" s="45"/>
+      <c r="R21" s="45"/>
+      <c r="S21" s="45"/>
+      <c r="T21" s="45"/>
+      <c r="U21" s="45"/>
+      <c r="V21" s="45"/>
+      <c r="W21" s="45"/>
+      <c r="X21" s="45"/>
+      <c r="Y21" s="45"/>
+      <c r="Z21" s="44"/>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="49" t="s">
+        <v>139</v>
+      </c>
+      <c r="B22" s="42"/>
+      <c r="C22" s="42"/>
+      <c r="D22" s="42"/>
+      <c r="E22" s="42"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
+      <c r="P22" s="45"/>
+      <c r="Q22" s="45"/>
+      <c r="R22" s="45"/>
+      <c r="S22" s="45"/>
+      <c r="T22" s="45"/>
+      <c r="U22" s="45"/>
+      <c r="V22" s="45"/>
+      <c r="W22" s="45"/>
+      <c r="X22" s="45"/>
+      <c r="Y22" s="45"/>
+      <c r="Z22" s="44"/>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="49" t="s">
+        <v>140</v>
+      </c>
+      <c r="B23" s="42"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="42"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
+      <c r="P23" s="45"/>
+      <c r="Q23" s="45"/>
+      <c r="R23" s="45"/>
+      <c r="S23" s="45"/>
+      <c r="T23" s="45"/>
+      <c r="U23" s="45"/>
+      <c r="V23" s="45"/>
+      <c r="W23" s="45"/>
+      <c r="X23" s="45"/>
+      <c r="Y23" s="45"/>
+      <c r="Z23" s="44"/>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" s="49" t="s">
+        <v>141</v>
+      </c>
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="42"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
+      <c r="P24" s="45"/>
+      <c r="Q24" s="45"/>
+      <c r="R24" s="45"/>
+      <c r="S24" s="45"/>
+      <c r="T24" s="45"/>
+      <c r="U24" s="45"/>
+      <c r="V24" s="45"/>
+      <c r="W24" s="45"/>
+      <c r="X24" s="45"/>
+      <c r="Y24" s="45"/>
+      <c r="Z24" s="44"/>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" s="49" t="s">
+        <v>142</v>
+      </c>
+      <c r="B25" s="42"/>
+      <c r="C25" s="42"/>
+      <c r="D25" s="42"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
+      <c r="P25" s="45"/>
+      <c r="Q25" s="45"/>
+      <c r="R25" s="45"/>
+      <c r="S25" s="45"/>
+      <c r="T25" s="45"/>
+      <c r="U25" s="45"/>
+      <c r="V25" s="45"/>
+      <c r="W25" s="45"/>
+      <c r="X25" s="45"/>
+      <c r="Y25" s="45"/>
+      <c r="Z25" s="44"/>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="42"/>
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42"/>
+      <c r="P26" s="45"/>
+      <c r="Q26" s="45"/>
+      <c r="R26" s="45"/>
+      <c r="S26" s="45"/>
+      <c r="T26" s="45"/>
+      <c r="U26" s="45"/>
+      <c r="V26" s="45"/>
+      <c r="W26" s="45"/>
+      <c r="X26" s="45"/>
+      <c r="Y26" s="45"/>
+      <c r="Z26" s="44"/>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" s="42"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="42"/>
+      <c r="P27" s="45"/>
+      <c r="Q27" s="45"/>
+      <c r="R27" s="45"/>
+      <c r="S27" s="45"/>
+      <c r="T27" s="45"/>
+      <c r="U27" s="45"/>
+      <c r="V27" s="45"/>
+      <c r="W27" s="45"/>
+      <c r="X27" s="45"/>
+      <c r="Y27" s="45"/>
+      <c r="Z27" s="44"/>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="42"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="42"/>
+      <c r="P28" s="45"/>
+      <c r="Q28" s="45"/>
+      <c r="R28" s="45"/>
+      <c r="S28" s="45"/>
+      <c r="T28" s="45"/>
+      <c r="U28" s="45"/>
+      <c r="V28" s="45"/>
+      <c r="W28" s="45"/>
+      <c r="X28" s="45"/>
+      <c r="Y28" s="45"/>
+      <c r="Z28" s="44"/>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="P29" s="45"/>
+      <c r="Q29" s="45"/>
+      <c r="R29" s="45"/>
+      <c r="S29" s="45"/>
+      <c r="T29" s="45"/>
+      <c r="U29" s="45"/>
+      <c r="V29" s="45"/>
+      <c r="W29" s="45"/>
+      <c r="X29" s="45"/>
+      <c r="Y29" s="45"/>
+      <c r="Z29" s="44"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="P5:Y5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:F69"/>
   <sheetViews>
@@ -2526,12 +3140,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" s="8" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="4" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
@@ -2581,156 +3195,156 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="30" t="s">
+      <c r="B10" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="31"/>
-      <c r="D10" s="31"/>
-      <c r="E10" s="31"/>
+      <c r="C10" s="38"/>
+      <c r="D10" s="38"/>
+      <c r="E10" s="38"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="26" t="s">
+      <c r="B11" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="26"/>
+      <c r="C11" s="29"/>
       <c r="D11" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E11" s="11"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="26" t="s">
+      <c r="B12" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="26"/>
+      <c r="C12" s="29"/>
       <c r="D12" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E12" s="11"/>
     </row>
     <row r="13" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="26" t="s">
+      <c r="B13" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="26"/>
+      <c r="C13" s="29"/>
       <c r="D13" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E13" s="11"/>
     </row>
     <row r="14" spans="2:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="26" t="s">
+      <c r="B14" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="26"/>
+      <c r="C14" s="29"/>
       <c r="D14" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E14" s="11"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="26"/>
+      <c r="C15" s="29"/>
       <c r="D15" s="10" t="s">
         <v>118</v>
       </c>
       <c r="E15" s="11"/>
     </row>
     <row r="16" spans="2:5" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="26" t="s">
+      <c r="B16" s="29" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="26"/>
+      <c r="C16" s="29"/>
       <c r="D16" s="10" t="s">
         <v>119</v>
       </c>
       <c r="E16" s="11"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="31"/>
+      <c r="C17" s="38"/>
+      <c r="D17" s="38"/>
+      <c r="E17" s="38"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="26" t="s">
+      <c r="B18" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="26"/>
+      <c r="C18" s="29"/>
       <c r="D18" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E18" s="11"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="26" t="s">
+      <c r="B19" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="26"/>
+      <c r="C19" s="29"/>
       <c r="D19" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E19" s="11"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="26" t="s">
+      <c r="B20" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="26"/>
+      <c r="C20" s="29"/>
       <c r="D20" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E20" s="11"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="26"/>
+      <c r="C21" s="29"/>
       <c r="D21" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E21" s="11"/>
     </row>
     <row r="22" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="26"/>
+      <c r="C22" s="29"/>
       <c r="D22" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E22" s="11"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="26" t="s">
+      <c r="B23" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="26"/>
+      <c r="C23" s="29"/>
       <c r="D23" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E23" s="11"/>
     </row>
     <row r="24" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="26" t="s">
+      <c r="B24" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="26"/>
+      <c r="C24" s="29"/>
       <c r="D24" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E24" s="11"/>
     </row>
     <row r="25" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="28" t="s">
+      <c r="B25" s="31" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="28"/>
+      <c r="C25" s="31"/>
       <c r="D25" s="23" t="s">
         <v>117</v>
       </c>
@@ -2745,20 +3359,20 @@
       <c r="E26" s="24"/>
     </row>
     <row r="27" spans="2:6" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="C27" s="28"/>
+      <c r="C27" s="31"/>
       <c r="D27" s="23" t="s">
         <v>117</v>
       </c>
       <c r="E27" s="24"/>
     </row>
     <row r="28" spans="2:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="36" t="s">
+      <c r="B28" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="C28" s="37"/>
+      <c r="C28" s="27"/>
       <c r="D28" s="10" t="s">
         <v>117</v>
       </c>
@@ -2768,10 +3382,10 @@
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="36" t="s">
+      <c r="B29" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="C29" s="37"/>
+      <c r="C29" s="27"/>
       <c r="D29" s="10" t="s">
         <v>117</v>
       </c>
@@ -2781,128 +3395,128 @@
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="28" t="s">
+      <c r="B30" s="31" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="28"/>
+      <c r="C30" s="31"/>
       <c r="D30" s="23" t="s">
         <v>117</v>
       </c>
       <c r="E30" s="24"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30"/>
+      <c r="E31" s="30"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="28" t="s">
+      <c r="B32" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="28"/>
+      <c r="C32" s="31"/>
       <c r="D32" s="23" t="s">
         <v>117</v>
       </c>
       <c r="E32" s="24"/>
     </row>
     <row r="33" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="28"/>
+      <c r="C33" s="31"/>
       <c r="D33" s="23" t="s">
         <v>117</v>
       </c>
       <c r="E33" s="24"/>
     </row>
     <row r="34" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="28"/>
+      <c r="C34" s="31"/>
       <c r="D34" s="23" t="s">
         <v>117</v>
       </c>
       <c r="E34" s="24"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="28" t="s">
+      <c r="B35" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="28"/>
+      <c r="C35" s="31"/>
       <c r="D35" s="23" t="s">
         <v>118</v>
       </c>
       <c r="E35" s="24"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="28" t="s">
+      <c r="B36" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="28"/>
+      <c r="C36" s="31"/>
       <c r="D36" s="23" t="s">
         <v>117</v>
       </c>
       <c r="E36" s="24"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="28" t="s">
+      <c r="B37" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="C37" s="28"/>
+      <c r="C37" s="31"/>
       <c r="D37" s="23" t="s">
         <v>117</v>
       </c>
       <c r="E37" s="24"/>
     </row>
     <row r="38" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="26" t="s">
+      <c r="B38" s="29" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="26"/>
+      <c r="C38" s="29"/>
       <c r="D38" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E38" s="11"/>
     </row>
     <row r="39" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="26" t="s">
+      <c r="B39" s="29" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="26"/>
+      <c r="C39" s="29"/>
       <c r="D39" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E39" s="11"/>
     </row>
     <row r="40" spans="2:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="26" t="s">
+      <c r="B40" s="29" t="s">
         <v>57</v>
       </c>
-      <c r="C40" s="26"/>
+      <c r="C40" s="29"/>
       <c r="D40" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E40" s="11"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="26" t="s">
+      <c r="B41" s="29" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="26"/>
+      <c r="C41" s="29"/>
       <c r="D41" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E41" s="11"/>
     </row>
     <row r="42" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="27" t="s">
+      <c r="B42" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="27"/>
+      <c r="C42" s="28"/>
       <c r="D42" s="10" t="s">
         <v>117</v>
       </c>
@@ -2912,170 +3526,170 @@
       </c>
     </row>
     <row r="43" spans="2:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="26" t="s">
+      <c r="B43" s="29" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="26"/>
+      <c r="C43" s="29"/>
       <c r="D43" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E43" s="11"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="26" t="s">
+      <c r="B44" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C44" s="26"/>
+      <c r="C44" s="29"/>
       <c r="D44" s="10" t="s">
         <v>119</v>
       </c>
       <c r="E44" s="11"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="26" t="s">
+      <c r="B45" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="26"/>
+      <c r="C45" s="29"/>
       <c r="D45" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E45" s="11"/>
     </row>
     <row r="46" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="26" t="s">
+      <c r="B46" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="26"/>
+      <c r="C46" s="29"/>
       <c r="D46" s="10" t="s">
         <v>118</v>
       </c>
       <c r="E46" s="11"/>
     </row>
     <row r="47" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="26" t="s">
+      <c r="B47" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="26"/>
+      <c r="C47" s="29"/>
       <c r="D47" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E47" s="11"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="26" t="s">
+      <c r="B48" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C48" s="26"/>
+      <c r="C48" s="29"/>
       <c r="D48" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E48" s="11"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C49" s="26"/>
+      <c r="C49" s="29"/>
       <c r="D49" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E49" s="11"/>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="26" t="s">
+      <c r="B50" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="C50" s="26"/>
+      <c r="C50" s="29"/>
       <c r="D50" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E50" s="11"/>
     </row>
     <row r="51" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="26" t="s">
+      <c r="B51" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="C51" s="26"/>
+      <c r="C51" s="29"/>
       <c r="D51" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E51" s="11"/>
     </row>
     <row r="52" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="26" t="s">
+      <c r="B52" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="C52" s="26"/>
+      <c r="C52" s="29"/>
       <c r="D52" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E52" s="11"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="26" t="s">
+      <c r="B53" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="C53" s="26"/>
+      <c r="C53" s="29"/>
       <c r="D53" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E53" s="11"/>
     </row>
     <row r="54" spans="2:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="27" t="s">
+      <c r="B54" s="28" t="s">
         <v>111</v>
       </c>
-      <c r="C54" s="27"/>
+      <c r="C54" s="28"/>
       <c r="D54" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E54" s="11"/>
     </row>
     <row r="55" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="26" t="s">
+      <c r="B55" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="C55" s="26"/>
+      <c r="C55" s="29"/>
       <c r="D55" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E55" s="11"/>
     </row>
     <row r="56" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="27" t="s">
+      <c r="B56" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="C56" s="27"/>
+      <c r="C56" s="28"/>
       <c r="D56" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E56" s="11"/>
     </row>
     <row r="57" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="27" t="s">
+      <c r="B57" s="28" t="s">
         <v>108</v>
       </c>
-      <c r="C57" s="27"/>
+      <c r="C57" s="28"/>
       <c r="D57" s="10" t="s">
         <v>119</v>
       </c>
       <c r="E57" s="11"/>
     </row>
     <row r="58" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="27" t="s">
+      <c r="B58" s="28" t="s">
         <v>109</v>
       </c>
-      <c r="C58" s="27"/>
+      <c r="C58" s="28"/>
       <c r="D58" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E58" s="11"/>
     </row>
     <row r="59" spans="2:6" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="27" t="s">
+      <c r="B59" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="C59" s="27"/>
+      <c r="C59" s="28"/>
       <c r="D59" s="10" t="s">
         <v>117</v>
       </c>
@@ -3146,32 +3760,6 @@
     </row>
   </sheetData>
   <mergeCells count="52">
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
@@ -3185,11 +3773,24 @@
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B9:C9"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B36:C36"/>
     <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
     <mergeCell ref="B55:C55"/>
     <mergeCell ref="B56:C56"/>
     <mergeCell ref="B57:C57"/>
@@ -3198,6 +3799,19 @@
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="B54:C54"/>
     <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B45:C45"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D65547:D65584 IU65547:IU65584 SQ65547:SQ65584 ACM65547:ACM65584 AMI65547:AMI65584 AWE65547:AWE65584 BGA65547:BGA65584 BPW65547:BPW65584 BZS65547:BZS65584 CJO65547:CJO65584 CTK65547:CTK65584 DDG65547:DDG65584 DNC65547:DNC65584 DWY65547:DWY65584 EGU65547:EGU65584 EQQ65547:EQQ65584 FAM65547:FAM65584 FKI65547:FKI65584 FUE65547:FUE65584 GEA65547:GEA65584 GNW65547:GNW65584 GXS65547:GXS65584 HHO65547:HHO65584 HRK65547:HRK65584 IBG65547:IBG65584 ILC65547:ILC65584 IUY65547:IUY65584 JEU65547:JEU65584 JOQ65547:JOQ65584 JYM65547:JYM65584 KII65547:KII65584 KSE65547:KSE65584 LCA65547:LCA65584 LLW65547:LLW65584 LVS65547:LVS65584 MFO65547:MFO65584 MPK65547:MPK65584 MZG65547:MZG65584 NJC65547:NJC65584 NSY65547:NSY65584 OCU65547:OCU65584 OMQ65547:OMQ65584 OWM65547:OWM65584 PGI65547:PGI65584 PQE65547:PQE65584 QAA65547:QAA65584 QJW65547:QJW65584 QTS65547:QTS65584 RDO65547:RDO65584 RNK65547:RNK65584 RXG65547:RXG65584 SHC65547:SHC65584 SQY65547:SQY65584 TAU65547:TAU65584 TKQ65547:TKQ65584 TUM65547:TUM65584 UEI65547:UEI65584 UOE65547:UOE65584 UYA65547:UYA65584 VHW65547:VHW65584 VRS65547:VRS65584 WBO65547:WBO65584 WLK65547:WLK65584 WVG65547:WVG65584 D131083:D131120 IU131083:IU131120 SQ131083:SQ131120 ACM131083:ACM131120 AMI131083:AMI131120 AWE131083:AWE131120 BGA131083:BGA131120 BPW131083:BPW131120 BZS131083:BZS131120 CJO131083:CJO131120 CTK131083:CTK131120 DDG131083:DDG131120 DNC131083:DNC131120 DWY131083:DWY131120 EGU131083:EGU131120 EQQ131083:EQQ131120 FAM131083:FAM131120 FKI131083:FKI131120 FUE131083:FUE131120 GEA131083:GEA131120 GNW131083:GNW131120 GXS131083:GXS131120 HHO131083:HHO131120 HRK131083:HRK131120 IBG131083:IBG131120 ILC131083:ILC131120 IUY131083:IUY131120 JEU131083:JEU131120 JOQ131083:JOQ131120 JYM131083:JYM131120 KII131083:KII131120 KSE131083:KSE131120 LCA131083:LCA131120 LLW131083:LLW131120 LVS131083:LVS131120 MFO131083:MFO131120 MPK131083:MPK131120 MZG131083:MZG131120 NJC131083:NJC131120 NSY131083:NSY131120 OCU131083:OCU131120 OMQ131083:OMQ131120 OWM131083:OWM131120 PGI131083:PGI131120 PQE131083:PQE131120 QAA131083:QAA131120 QJW131083:QJW131120 QTS131083:QTS131120 RDO131083:RDO131120 RNK131083:RNK131120 RXG131083:RXG131120 SHC131083:SHC131120 SQY131083:SQY131120 TAU131083:TAU131120 TKQ131083:TKQ131120 TUM131083:TUM131120 UEI131083:UEI131120 UOE131083:UOE131120 UYA131083:UYA131120 VHW131083:VHW131120 VRS131083:VRS131120 WBO131083:WBO131120 WLK131083:WLK131120 WVG131083:WVG131120 D196619:D196656 IU196619:IU196656 SQ196619:SQ196656 ACM196619:ACM196656 AMI196619:AMI196656 AWE196619:AWE196656 BGA196619:BGA196656 BPW196619:BPW196656 BZS196619:BZS196656 CJO196619:CJO196656 CTK196619:CTK196656 DDG196619:DDG196656 DNC196619:DNC196656 DWY196619:DWY196656 EGU196619:EGU196656 EQQ196619:EQQ196656 FAM196619:FAM196656 FKI196619:FKI196656 FUE196619:FUE196656 GEA196619:GEA196656 GNW196619:GNW196656 GXS196619:GXS196656 HHO196619:HHO196656 HRK196619:HRK196656 IBG196619:IBG196656 ILC196619:ILC196656 IUY196619:IUY196656 JEU196619:JEU196656 JOQ196619:JOQ196656 JYM196619:JYM196656 KII196619:KII196656 KSE196619:KSE196656 LCA196619:LCA196656 LLW196619:LLW196656 LVS196619:LVS196656 MFO196619:MFO196656 MPK196619:MPK196656 MZG196619:MZG196656 NJC196619:NJC196656 NSY196619:NSY196656 OCU196619:OCU196656 OMQ196619:OMQ196656 OWM196619:OWM196656 PGI196619:PGI196656 PQE196619:PQE196656 QAA196619:QAA196656 QJW196619:QJW196656 QTS196619:QTS196656 RDO196619:RDO196656 RNK196619:RNK196656 RXG196619:RXG196656 SHC196619:SHC196656 SQY196619:SQY196656 TAU196619:TAU196656 TKQ196619:TKQ196656 TUM196619:TUM196656 UEI196619:UEI196656 UOE196619:UOE196656 UYA196619:UYA196656 VHW196619:VHW196656 VRS196619:VRS196656 WBO196619:WBO196656 WLK196619:WLK196656 WVG196619:WVG196656 D262155:D262192 IU262155:IU262192 SQ262155:SQ262192 ACM262155:ACM262192 AMI262155:AMI262192 AWE262155:AWE262192 BGA262155:BGA262192 BPW262155:BPW262192 BZS262155:BZS262192 CJO262155:CJO262192 CTK262155:CTK262192 DDG262155:DDG262192 DNC262155:DNC262192 DWY262155:DWY262192 EGU262155:EGU262192 EQQ262155:EQQ262192 FAM262155:FAM262192 FKI262155:FKI262192 FUE262155:FUE262192 GEA262155:GEA262192 GNW262155:GNW262192 GXS262155:GXS262192 HHO262155:HHO262192 HRK262155:HRK262192 IBG262155:IBG262192 ILC262155:ILC262192 IUY262155:IUY262192 JEU262155:JEU262192 JOQ262155:JOQ262192 JYM262155:JYM262192 KII262155:KII262192 KSE262155:KSE262192 LCA262155:LCA262192 LLW262155:LLW262192 LVS262155:LVS262192 MFO262155:MFO262192 MPK262155:MPK262192 MZG262155:MZG262192 NJC262155:NJC262192 NSY262155:NSY262192 OCU262155:OCU262192 OMQ262155:OMQ262192 OWM262155:OWM262192 PGI262155:PGI262192 PQE262155:PQE262192 QAA262155:QAA262192 QJW262155:QJW262192 QTS262155:QTS262192 RDO262155:RDO262192 RNK262155:RNK262192 RXG262155:RXG262192 SHC262155:SHC262192 SQY262155:SQY262192 TAU262155:TAU262192 TKQ262155:TKQ262192 TUM262155:TUM262192 UEI262155:UEI262192 UOE262155:UOE262192 UYA262155:UYA262192 VHW262155:VHW262192 VRS262155:VRS262192 WBO262155:WBO262192 WLK262155:WLK262192 WVG262155:WVG262192 D327691:D327728 IU327691:IU327728 SQ327691:SQ327728 ACM327691:ACM327728 AMI327691:AMI327728 AWE327691:AWE327728 BGA327691:BGA327728 BPW327691:BPW327728 BZS327691:BZS327728 CJO327691:CJO327728 CTK327691:CTK327728 DDG327691:DDG327728 DNC327691:DNC327728 DWY327691:DWY327728 EGU327691:EGU327728 EQQ327691:EQQ327728 FAM327691:FAM327728 FKI327691:FKI327728 FUE327691:FUE327728 GEA327691:GEA327728 GNW327691:GNW327728 GXS327691:GXS327728 HHO327691:HHO327728 HRK327691:HRK327728 IBG327691:IBG327728 ILC327691:ILC327728 IUY327691:IUY327728 JEU327691:JEU327728 JOQ327691:JOQ327728 JYM327691:JYM327728 KII327691:KII327728 KSE327691:KSE327728 LCA327691:LCA327728 LLW327691:LLW327728 LVS327691:LVS327728 MFO327691:MFO327728 MPK327691:MPK327728 MZG327691:MZG327728 NJC327691:NJC327728 NSY327691:NSY327728 OCU327691:OCU327728 OMQ327691:OMQ327728 OWM327691:OWM327728 PGI327691:PGI327728 PQE327691:PQE327728 QAA327691:QAA327728 QJW327691:QJW327728 QTS327691:QTS327728 RDO327691:RDO327728 RNK327691:RNK327728 RXG327691:RXG327728 SHC327691:SHC327728 SQY327691:SQY327728 TAU327691:TAU327728 TKQ327691:TKQ327728 TUM327691:TUM327728 UEI327691:UEI327728 UOE327691:UOE327728 UYA327691:UYA327728 VHW327691:VHW327728 VRS327691:VRS327728 WBO327691:WBO327728 WLK327691:WLK327728 WVG327691:WVG327728 D393227:D393264 IU393227:IU393264 SQ393227:SQ393264 ACM393227:ACM393264 AMI393227:AMI393264 AWE393227:AWE393264 BGA393227:BGA393264 BPW393227:BPW393264 BZS393227:BZS393264 CJO393227:CJO393264 CTK393227:CTK393264 DDG393227:DDG393264 DNC393227:DNC393264 DWY393227:DWY393264 EGU393227:EGU393264 EQQ393227:EQQ393264 FAM393227:FAM393264 FKI393227:FKI393264 FUE393227:FUE393264 GEA393227:GEA393264 GNW393227:GNW393264 GXS393227:GXS393264 HHO393227:HHO393264 HRK393227:HRK393264 IBG393227:IBG393264 ILC393227:ILC393264 IUY393227:IUY393264 JEU393227:JEU393264 JOQ393227:JOQ393264 JYM393227:JYM393264 KII393227:KII393264 KSE393227:KSE393264 LCA393227:LCA393264 LLW393227:LLW393264 LVS393227:LVS393264 MFO393227:MFO393264 MPK393227:MPK393264 MZG393227:MZG393264 NJC393227:NJC393264 NSY393227:NSY393264 OCU393227:OCU393264 OMQ393227:OMQ393264 OWM393227:OWM393264 PGI393227:PGI393264 PQE393227:PQE393264 QAA393227:QAA393264 QJW393227:QJW393264 QTS393227:QTS393264 RDO393227:RDO393264 RNK393227:RNK393264 RXG393227:RXG393264 SHC393227:SHC393264 SQY393227:SQY393264 TAU393227:TAU393264 TKQ393227:TKQ393264 TUM393227:TUM393264 UEI393227:UEI393264 UOE393227:UOE393264 UYA393227:UYA393264 VHW393227:VHW393264 VRS393227:VRS393264 WBO393227:WBO393264 WLK393227:WLK393264 WVG393227:WVG393264 D458763:D458800 IU458763:IU458800 SQ458763:SQ458800 ACM458763:ACM458800 AMI458763:AMI458800 AWE458763:AWE458800 BGA458763:BGA458800 BPW458763:BPW458800 BZS458763:BZS458800 CJO458763:CJO458800 CTK458763:CTK458800 DDG458763:DDG458800 DNC458763:DNC458800 DWY458763:DWY458800 EGU458763:EGU458800 EQQ458763:EQQ458800 FAM458763:FAM458800 FKI458763:FKI458800 FUE458763:FUE458800 GEA458763:GEA458800 GNW458763:GNW458800 GXS458763:GXS458800 HHO458763:HHO458800 HRK458763:HRK458800 IBG458763:IBG458800 ILC458763:ILC458800 IUY458763:IUY458800 JEU458763:JEU458800 JOQ458763:JOQ458800 JYM458763:JYM458800 KII458763:KII458800 KSE458763:KSE458800 LCA458763:LCA458800 LLW458763:LLW458800 LVS458763:LVS458800 MFO458763:MFO458800 MPK458763:MPK458800 MZG458763:MZG458800 NJC458763:NJC458800 NSY458763:NSY458800 OCU458763:OCU458800 OMQ458763:OMQ458800 OWM458763:OWM458800 PGI458763:PGI458800 PQE458763:PQE458800 QAA458763:QAA458800 QJW458763:QJW458800 QTS458763:QTS458800 RDO458763:RDO458800 RNK458763:RNK458800 RXG458763:RXG458800 SHC458763:SHC458800 SQY458763:SQY458800 TAU458763:TAU458800 TKQ458763:TKQ458800 TUM458763:TUM458800 UEI458763:UEI458800 UOE458763:UOE458800 UYA458763:UYA458800 VHW458763:VHW458800 VRS458763:VRS458800 WBO458763:WBO458800 WLK458763:WLK458800 WVG458763:WVG458800 D524299:D524336 IU524299:IU524336 SQ524299:SQ524336 ACM524299:ACM524336 AMI524299:AMI524336 AWE524299:AWE524336 BGA524299:BGA524336 BPW524299:BPW524336 BZS524299:BZS524336 CJO524299:CJO524336 CTK524299:CTK524336 DDG524299:DDG524336 DNC524299:DNC524336 DWY524299:DWY524336 EGU524299:EGU524336 EQQ524299:EQQ524336 FAM524299:FAM524336 FKI524299:FKI524336 FUE524299:FUE524336 GEA524299:GEA524336 GNW524299:GNW524336 GXS524299:GXS524336 HHO524299:HHO524336 HRK524299:HRK524336 IBG524299:IBG524336 ILC524299:ILC524336 IUY524299:IUY524336 JEU524299:JEU524336 JOQ524299:JOQ524336 JYM524299:JYM524336 KII524299:KII524336 KSE524299:KSE524336 LCA524299:LCA524336 LLW524299:LLW524336 LVS524299:LVS524336 MFO524299:MFO524336 MPK524299:MPK524336 MZG524299:MZG524336 NJC524299:NJC524336 NSY524299:NSY524336 OCU524299:OCU524336 OMQ524299:OMQ524336 OWM524299:OWM524336 PGI524299:PGI524336 PQE524299:PQE524336 QAA524299:QAA524336 QJW524299:QJW524336 QTS524299:QTS524336 RDO524299:RDO524336 RNK524299:RNK524336 RXG524299:RXG524336 SHC524299:SHC524336 SQY524299:SQY524336 TAU524299:TAU524336 TKQ524299:TKQ524336 TUM524299:TUM524336 UEI524299:UEI524336 UOE524299:UOE524336 UYA524299:UYA524336 VHW524299:VHW524336 VRS524299:VRS524336 WBO524299:WBO524336 WLK524299:WLK524336 WVG524299:WVG524336 D589835:D589872 IU589835:IU589872 SQ589835:SQ589872 ACM589835:ACM589872 AMI589835:AMI589872 AWE589835:AWE589872 BGA589835:BGA589872 BPW589835:BPW589872 BZS589835:BZS589872 CJO589835:CJO589872 CTK589835:CTK589872 DDG589835:DDG589872 DNC589835:DNC589872 DWY589835:DWY589872 EGU589835:EGU589872 EQQ589835:EQQ589872 FAM589835:FAM589872 FKI589835:FKI589872 FUE589835:FUE589872 GEA589835:GEA589872 GNW589835:GNW589872 GXS589835:GXS589872 HHO589835:HHO589872 HRK589835:HRK589872 IBG589835:IBG589872 ILC589835:ILC589872 IUY589835:IUY589872 JEU589835:JEU589872 JOQ589835:JOQ589872 JYM589835:JYM589872 KII589835:KII589872 KSE589835:KSE589872 LCA589835:LCA589872 LLW589835:LLW589872 LVS589835:LVS589872 MFO589835:MFO589872 MPK589835:MPK589872 MZG589835:MZG589872 NJC589835:NJC589872 NSY589835:NSY589872 OCU589835:OCU589872 OMQ589835:OMQ589872 OWM589835:OWM589872 PGI589835:PGI589872 PQE589835:PQE589872 QAA589835:QAA589872 QJW589835:QJW589872 QTS589835:QTS589872 RDO589835:RDO589872 RNK589835:RNK589872 RXG589835:RXG589872 SHC589835:SHC589872 SQY589835:SQY589872 TAU589835:TAU589872 TKQ589835:TKQ589872 TUM589835:TUM589872 UEI589835:UEI589872 UOE589835:UOE589872 UYA589835:UYA589872 VHW589835:VHW589872 VRS589835:VRS589872 WBO589835:WBO589872 WLK589835:WLK589872 WVG589835:WVG589872 D655371:D655408 IU655371:IU655408 SQ655371:SQ655408 ACM655371:ACM655408 AMI655371:AMI655408 AWE655371:AWE655408 BGA655371:BGA655408 BPW655371:BPW655408 BZS655371:BZS655408 CJO655371:CJO655408 CTK655371:CTK655408 DDG655371:DDG655408 DNC655371:DNC655408 DWY655371:DWY655408 EGU655371:EGU655408 EQQ655371:EQQ655408 FAM655371:FAM655408 FKI655371:FKI655408 FUE655371:FUE655408 GEA655371:GEA655408 GNW655371:GNW655408 GXS655371:GXS655408 HHO655371:HHO655408 HRK655371:HRK655408 IBG655371:IBG655408 ILC655371:ILC655408 IUY655371:IUY655408 JEU655371:JEU655408 JOQ655371:JOQ655408 JYM655371:JYM655408 KII655371:KII655408 KSE655371:KSE655408 LCA655371:LCA655408 LLW655371:LLW655408 LVS655371:LVS655408 MFO655371:MFO655408 MPK655371:MPK655408 MZG655371:MZG655408 NJC655371:NJC655408 NSY655371:NSY655408 OCU655371:OCU655408 OMQ655371:OMQ655408 OWM655371:OWM655408 PGI655371:PGI655408 PQE655371:PQE655408 QAA655371:QAA655408 QJW655371:QJW655408 QTS655371:QTS655408 RDO655371:RDO655408 RNK655371:RNK655408 RXG655371:RXG655408 SHC655371:SHC655408 SQY655371:SQY655408 TAU655371:TAU655408 TKQ655371:TKQ655408 TUM655371:TUM655408 UEI655371:UEI655408 UOE655371:UOE655408 UYA655371:UYA655408 VHW655371:VHW655408 VRS655371:VRS655408 WBO655371:WBO655408 WLK655371:WLK655408 WVG655371:WVG655408 D720907:D720944 IU720907:IU720944 SQ720907:SQ720944 ACM720907:ACM720944 AMI720907:AMI720944 AWE720907:AWE720944 BGA720907:BGA720944 BPW720907:BPW720944 BZS720907:BZS720944 CJO720907:CJO720944 CTK720907:CTK720944 DDG720907:DDG720944 DNC720907:DNC720944 DWY720907:DWY720944 EGU720907:EGU720944 EQQ720907:EQQ720944 FAM720907:FAM720944 FKI720907:FKI720944 FUE720907:FUE720944 GEA720907:GEA720944 GNW720907:GNW720944 GXS720907:GXS720944 HHO720907:HHO720944 HRK720907:HRK720944 IBG720907:IBG720944 ILC720907:ILC720944 IUY720907:IUY720944 JEU720907:JEU720944 JOQ720907:JOQ720944 JYM720907:JYM720944 KII720907:KII720944 KSE720907:KSE720944 LCA720907:LCA720944 LLW720907:LLW720944 LVS720907:LVS720944 MFO720907:MFO720944 MPK720907:MPK720944 MZG720907:MZG720944 NJC720907:NJC720944 NSY720907:NSY720944 OCU720907:OCU720944 OMQ720907:OMQ720944 OWM720907:OWM720944 PGI720907:PGI720944 PQE720907:PQE720944 QAA720907:QAA720944 QJW720907:QJW720944 QTS720907:QTS720944 RDO720907:RDO720944 RNK720907:RNK720944 RXG720907:RXG720944 SHC720907:SHC720944 SQY720907:SQY720944 TAU720907:TAU720944 TKQ720907:TKQ720944 TUM720907:TUM720944 UEI720907:UEI720944 UOE720907:UOE720944 UYA720907:UYA720944 VHW720907:VHW720944 VRS720907:VRS720944 WBO720907:WBO720944 WLK720907:WLK720944 WVG720907:WVG720944 D786443:D786480 IU786443:IU786480 SQ786443:SQ786480 ACM786443:ACM786480 AMI786443:AMI786480 AWE786443:AWE786480 BGA786443:BGA786480 BPW786443:BPW786480 BZS786443:BZS786480 CJO786443:CJO786480 CTK786443:CTK786480 DDG786443:DDG786480 DNC786443:DNC786480 DWY786443:DWY786480 EGU786443:EGU786480 EQQ786443:EQQ786480 FAM786443:FAM786480 FKI786443:FKI786480 FUE786443:FUE786480 GEA786443:GEA786480 GNW786443:GNW786480 GXS786443:GXS786480 HHO786443:HHO786480 HRK786443:HRK786480 IBG786443:IBG786480 ILC786443:ILC786480 IUY786443:IUY786480 JEU786443:JEU786480 JOQ786443:JOQ786480 JYM786443:JYM786480 KII786443:KII786480 KSE786443:KSE786480 LCA786443:LCA786480 LLW786443:LLW786480 LVS786443:LVS786480 MFO786443:MFO786480 MPK786443:MPK786480 MZG786443:MZG786480 NJC786443:NJC786480 NSY786443:NSY786480 OCU786443:OCU786480 OMQ786443:OMQ786480 OWM786443:OWM786480 PGI786443:PGI786480 PQE786443:PQE786480 QAA786443:QAA786480 QJW786443:QJW786480 QTS786443:QTS786480 RDO786443:RDO786480 RNK786443:RNK786480 RXG786443:RXG786480 SHC786443:SHC786480 SQY786443:SQY786480 TAU786443:TAU786480 TKQ786443:TKQ786480 TUM786443:TUM786480 UEI786443:UEI786480 UOE786443:UOE786480 UYA786443:UYA786480 VHW786443:VHW786480 VRS786443:VRS786480 WBO786443:WBO786480 WLK786443:WLK786480 WVG786443:WVG786480 D851979:D852016 IU851979:IU852016 SQ851979:SQ852016 ACM851979:ACM852016 AMI851979:AMI852016 AWE851979:AWE852016 BGA851979:BGA852016 BPW851979:BPW852016 BZS851979:BZS852016 CJO851979:CJO852016 CTK851979:CTK852016 DDG851979:DDG852016 DNC851979:DNC852016 DWY851979:DWY852016 EGU851979:EGU852016 EQQ851979:EQQ852016 FAM851979:FAM852016 FKI851979:FKI852016 FUE851979:FUE852016 GEA851979:GEA852016 GNW851979:GNW852016 GXS851979:GXS852016 HHO851979:HHO852016 HRK851979:HRK852016 IBG851979:IBG852016 ILC851979:ILC852016 IUY851979:IUY852016 JEU851979:JEU852016 JOQ851979:JOQ852016 JYM851979:JYM852016 KII851979:KII852016 KSE851979:KSE852016 LCA851979:LCA852016 LLW851979:LLW852016 LVS851979:LVS852016 MFO851979:MFO852016 MPK851979:MPK852016 MZG851979:MZG852016 NJC851979:NJC852016 NSY851979:NSY852016 OCU851979:OCU852016 OMQ851979:OMQ852016 OWM851979:OWM852016 PGI851979:PGI852016 PQE851979:PQE852016 QAA851979:QAA852016 QJW851979:QJW852016 QTS851979:QTS852016 RDO851979:RDO852016 RNK851979:RNK852016 RXG851979:RXG852016 SHC851979:SHC852016 SQY851979:SQY852016 TAU851979:TAU852016 TKQ851979:TKQ852016 TUM851979:TUM852016 UEI851979:UEI852016 UOE851979:UOE852016 UYA851979:UYA852016 VHW851979:VHW852016 VRS851979:VRS852016 WBO851979:WBO852016 WLK851979:WLK852016 WVG851979:WVG852016 D917515:D917552 IU917515:IU917552 SQ917515:SQ917552 ACM917515:ACM917552 AMI917515:AMI917552 AWE917515:AWE917552 BGA917515:BGA917552 BPW917515:BPW917552 BZS917515:BZS917552 CJO917515:CJO917552 CTK917515:CTK917552 DDG917515:DDG917552 DNC917515:DNC917552 DWY917515:DWY917552 EGU917515:EGU917552 EQQ917515:EQQ917552 FAM917515:FAM917552 FKI917515:FKI917552 FUE917515:FUE917552 GEA917515:GEA917552 GNW917515:GNW917552 GXS917515:GXS917552 HHO917515:HHO917552 HRK917515:HRK917552 IBG917515:IBG917552 ILC917515:ILC917552 IUY917515:IUY917552 JEU917515:JEU917552 JOQ917515:JOQ917552 JYM917515:JYM917552 KII917515:KII917552 KSE917515:KSE917552 LCA917515:LCA917552 LLW917515:LLW917552 LVS917515:LVS917552 MFO917515:MFO917552 MPK917515:MPK917552 MZG917515:MZG917552 NJC917515:NJC917552 NSY917515:NSY917552 OCU917515:OCU917552 OMQ917515:OMQ917552 OWM917515:OWM917552 PGI917515:PGI917552 PQE917515:PQE917552 QAA917515:QAA917552 QJW917515:QJW917552 QTS917515:QTS917552 RDO917515:RDO917552 RNK917515:RNK917552 RXG917515:RXG917552 SHC917515:SHC917552 SQY917515:SQY917552 TAU917515:TAU917552 TKQ917515:TKQ917552 TUM917515:TUM917552 UEI917515:UEI917552 UOE917515:UOE917552 UYA917515:UYA917552 VHW917515:VHW917552 VRS917515:VRS917552 WBO917515:WBO917552 WLK917515:WLK917552 WVG917515:WVG917552 D983051:D983088 IU983051:IU983088 SQ983051:SQ983088 ACM983051:ACM983088 AMI983051:AMI983088 AWE983051:AWE983088 BGA983051:BGA983088 BPW983051:BPW983088 BZS983051:BZS983088 CJO983051:CJO983088 CTK983051:CTK983088 DDG983051:DDG983088 DNC983051:DNC983088 DWY983051:DWY983088 EGU983051:EGU983088 EQQ983051:EQQ983088 FAM983051:FAM983088 FKI983051:FKI983088 FUE983051:FUE983088 GEA983051:GEA983088 GNW983051:GNW983088 GXS983051:GXS983088 HHO983051:HHO983088 HRK983051:HRK983088 IBG983051:IBG983088 ILC983051:ILC983088 IUY983051:IUY983088 JEU983051:JEU983088 JOQ983051:JOQ983088 JYM983051:JYM983088 KII983051:KII983088 KSE983051:KSE983088 LCA983051:LCA983088 LLW983051:LLW983088 LVS983051:LVS983088 MFO983051:MFO983088 MPK983051:MPK983088 MZG983051:MZG983088 NJC983051:NJC983088 NSY983051:NSY983088 OCU983051:OCU983088 OMQ983051:OMQ983088 OWM983051:OWM983088 PGI983051:PGI983088 PQE983051:PQE983088 QAA983051:QAA983088 QJW983051:QJW983088 QTS983051:QTS983088 RDO983051:RDO983088 RNK983051:RNK983088 RXG983051:RXG983088 SHC983051:SHC983088 SQY983051:SQY983088 TAU983051:TAU983088 TKQ983051:TKQ983088 TUM983051:TUM983088 UEI983051:UEI983088 UOE983051:UOE983088 UYA983051:UYA983088 VHW983051:VHW983088 VRS983051:VRS983088 WBO983051:WBO983088 WLK983051:WLK983088 WVG983051:WVG983088 D11:D16 D18:D59 WBO11:WBO59 VRS11:VRS59 VHW11:VHW59 UYA11:UYA59 UOE11:UOE59 UEI11:UEI59 TUM11:TUM59 TKQ11:TKQ59 TAU11:TAU59 SQY11:SQY59 SHC11:SHC59 RXG11:RXG59 RNK11:RNK59 RDO11:RDO59 QTS11:QTS59 QJW11:QJW59 QAA11:QAA59 PQE11:PQE59 PGI11:PGI59 OWM11:OWM59 OMQ11:OMQ59 OCU11:OCU59 NSY11:NSY59 NJC11:NJC59 MZG11:MZG59 MPK11:MPK59 MFO11:MFO59 LVS11:LVS59 LLW11:LLW59 LCA11:LCA59 KSE11:KSE59 KII11:KII59 JYM11:JYM59 JOQ11:JOQ59 JEU11:JEU59 IUY11:IUY59 ILC11:ILC59 IBG11:IBG59 HRK11:HRK59 HHO11:HHO59 GXS11:GXS59 GNW11:GNW59 GEA11:GEA59 FUE11:FUE59 FKI11:FKI59 FAM11:FAM59 EQQ11:EQQ59 EGU11:EGU59 DWY11:DWY59 DNC11:DNC59 DDG11:DDG59 CTK11:CTK59 CJO11:CJO59 BZS11:BZS59 BPW11:BPW59 BGA11:BGA59 AWE11:AWE59 AMI11:AMI59 ACM11:ACM59 SQ11:SQ59 IU11:IU59 WLK11:WLK59 WVG11:WVG59" xr:uid="{00000000-0002-0000-0200-000000000000}">
@@ -3213,7 +3827,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
@@ -3524,7 +4138,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:E29"/>
   <sheetViews>
@@ -3757,7 +4371,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:A6"/>
   <sheetViews>

</xml_diff>

<commit_message>
#feat: update checklist and rule
</commit_message>
<xml_diff>
--- a/docs/specs/Checklist.xlsx
+++ b/docs/specs/Checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Template Source\VUE\vue-mocha\docs\specs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0630F225-2B75-4BD0-913B-A506C9115A9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F89CBF9-1AF4-4A46-8A81-9D1501E9EA13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -191,7 +191,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="144">
   <si>
     <t>Question</t>
   </si>
@@ -657,6 +657,9 @@
   </si>
   <si>
     <t>- Tham khảo cấu trúc thư mục hiện tại để làm theo</t>
+  </si>
+  <si>
+    <t>- Api sử dụng mockapi.io để làm =&gt; copy url của mockapi.io bỏ vào file .env để sử dụng</t>
   </si>
 </sst>
 </file>
@@ -876,7 +879,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -947,77 +950,68 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -2219,522 +2213,241 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14A85404-3A40-4CA2-8D80-1BD7AEC101DF}">
-  <dimension ref="A2:Z29"/>
+  <dimension ref="A2:Y28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.140625" style="39"/>
+    <col min="1" max="16384" width="9.140625" style="26"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="41" t="s">
+    <row r="2" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="28" t="s">
         <v>128</v>
       </c>
-      <c r="P2" s="45"/>
-      <c r="Q2" s="45"/>
-      <c r="R2" s="45"/>
-      <c r="S2" s="45"/>
-      <c r="T2" s="45"/>
-      <c r="U2" s="45"/>
-      <c r="V2" s="45"/>
-      <c r="W2" s="45"/>
-      <c r="X2" s="45"/>
-      <c r="Y2" s="45"/>
-      <c r="Z2" s="43"/>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B3" s="40" t="s">
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="26"/>
+    </row>
+    <row r="3" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B3" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="P3" s="45"/>
-      <c r="Q3" s="46"/>
-      <c r="R3" s="45"/>
-      <c r="S3" s="45"/>
-      <c r="T3" s="45"/>
-      <c r="U3" s="45"/>
-      <c r="V3" s="45"/>
-      <c r="W3" s="45"/>
-      <c r="X3" s="45"/>
-      <c r="Y3" s="45"/>
-      <c r="Z3" s="44"/>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B4" s="40" t="s">
+      <c r="Q3" s="30"/>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B4" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="P4" s="45"/>
-      <c r="Q4" s="45"/>
-      <c r="R4" s="45"/>
-      <c r="S4" s="45"/>
-      <c r="T4" s="45"/>
-      <c r="U4" s="45"/>
-      <c r="V4" s="45"/>
-      <c r="W4" s="45"/>
-      <c r="X4" s="45"/>
-      <c r="Y4" s="45"/>
-      <c r="Z4" s="44"/>
-    </row>
-    <row r="5" spans="1:26" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="40" t="s">
+    </row>
+    <row r="5" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="P5" s="47"/>
-      <c r="Q5" s="48"/>
-      <c r="R5" s="48"/>
-      <c r="S5" s="48"/>
-      <c r="T5" s="48"/>
-      <c r="U5" s="48"/>
-      <c r="V5" s="48"/>
-      <c r="W5" s="48"/>
-      <c r="X5" s="48"/>
-      <c r="Y5" s="48"/>
-      <c r="Z5" s="44"/>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="P6" s="45"/>
-      <c r="Q6" s="45"/>
-      <c r="R6" s="45"/>
-      <c r="S6" s="45"/>
-      <c r="T6" s="45"/>
-      <c r="U6" s="45"/>
-      <c r="V6" s="45"/>
-      <c r="W6" s="45"/>
-      <c r="X6" s="45"/>
-      <c r="Y6" s="45"/>
-      <c r="Z6" s="44"/>
-    </row>
-    <row r="7" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="41" t="s">
+      <c r="P5" s="32"/>
+      <c r="Q5" s="33"/>
+      <c r="R5" s="33"/>
+      <c r="S5" s="33"/>
+      <c r="T5" s="33"/>
+      <c r="U5" s="33"/>
+      <c r="V5" s="33"/>
+      <c r="W5" s="33"/>
+      <c r="X5" s="33"/>
+      <c r="Y5" s="33"/>
+    </row>
+    <row r="7" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
         <v>131</v>
       </c>
-      <c r="P7" s="45"/>
-      <c r="Q7" s="45"/>
-      <c r="R7" s="45"/>
-      <c r="S7" s="45"/>
-      <c r="T7" s="45"/>
-      <c r="U7" s="45"/>
-      <c r="V7" s="45"/>
-      <c r="W7" s="45"/>
-      <c r="X7" s="45"/>
-      <c r="Y7" s="45"/>
-      <c r="Z7" s="43"/>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B8" s="40" t="s">
+      <c r="P7" s="26"/>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="26"/>
+      <c r="S7" s="26"/>
+      <c r="T7" s="26"/>
+      <c r="U7" s="26"/>
+      <c r="V7" s="26"/>
+      <c r="W7" s="26"/>
+      <c r="X7" s="26"/>
+      <c r="Y7" s="26"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B8" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="P8" s="45"/>
-      <c r="Q8" s="45"/>
-      <c r="R8" s="45"/>
-      <c r="S8" s="45"/>
-      <c r="T8" s="45"/>
-      <c r="U8" s="45"/>
-      <c r="V8" s="45"/>
-      <c r="W8" s="45"/>
-      <c r="X8" s="45"/>
-      <c r="Y8" s="45"/>
-      <c r="Z8" s="44"/>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B9" s="40" t="s">
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B9" s="27" t="s">
         <v>133</v>
       </c>
-      <c r="P9" s="45"/>
-      <c r="Q9" s="45"/>
-      <c r="R9" s="45"/>
-      <c r="S9" s="45"/>
-      <c r="T9" s="45"/>
-      <c r="U9" s="45"/>
-      <c r="V9" s="45"/>
-      <c r="W9" s="45"/>
-      <c r="X9" s="45"/>
-      <c r="Y9" s="45"/>
-      <c r="Z9" s="44"/>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B10" s="40"/>
-      <c r="P10" s="45"/>
-      <c r="Q10" s="45"/>
-      <c r="R10" s="45"/>
-      <c r="S10" s="45"/>
-      <c r="T10" s="45"/>
-      <c r="U10" s="45"/>
-      <c r="V10" s="45"/>
-      <c r="W10" s="45"/>
-      <c r="X10" s="45"/>
-      <c r="Y10" s="45"/>
-      <c r="Z10" s="44"/>
-    </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="P11" s="45"/>
-      <c r="Q11" s="45"/>
-      <c r="R11" s="45"/>
-      <c r="S11" s="45"/>
-      <c r="T11" s="45"/>
-      <c r="U11" s="45"/>
-      <c r="V11" s="45"/>
-      <c r="W11" s="45"/>
-      <c r="X11" s="45"/>
-      <c r="Y11" s="45"/>
-      <c r="Z11" s="44"/>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="P12" s="45"/>
-      <c r="Q12" s="45"/>
-      <c r="R12" s="45"/>
-      <c r="S12" s="45"/>
-      <c r="T12" s="45"/>
-      <c r="U12" s="45"/>
-      <c r="V12" s="45"/>
-      <c r="W12" s="45"/>
-      <c r="X12" s="45"/>
-      <c r="Y12" s="45"/>
-      <c r="Z12" s="44"/>
-    </row>
-    <row r="13" spans="1:26" s="41" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="41" t="s">
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B10" s="27"/>
+    </row>
+    <row r="13" spans="1:25" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="P13" s="45"/>
-      <c r="Q13" s="45"/>
-      <c r="R13" s="45"/>
-      <c r="S13" s="45"/>
-      <c r="T13" s="45"/>
-      <c r="U13" s="45"/>
-      <c r="V13" s="45"/>
-      <c r="W13" s="45"/>
-      <c r="X13" s="45"/>
-      <c r="Y13" s="45"/>
-      <c r="Z13" s="43"/>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B14" s="40" t="s">
+      <c r="P13" s="26"/>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="26"/>
+      <c r="S13" s="26"/>
+      <c r="T13" s="26"/>
+      <c r="U13" s="26"/>
+      <c r="V13" s="26"/>
+      <c r="W13" s="26"/>
+      <c r="X13" s="26"/>
+      <c r="Y13" s="26"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B14" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="P14" s="45"/>
-      <c r="Q14" s="45"/>
-      <c r="R14" s="45"/>
-      <c r="S14" s="45"/>
-      <c r="T14" s="45"/>
-      <c r="U14" s="45"/>
-      <c r="V14" s="45"/>
-      <c r="W14" s="45"/>
-      <c r="X14" s="45"/>
-      <c r="Y14" s="45"/>
-      <c r="Z14" s="44"/>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="B15" s="40" t="s">
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="B15" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="P15" s="45"/>
-      <c r="Q15" s="45"/>
-      <c r="R15" s="45"/>
-      <c r="S15" s="45"/>
-      <c r="T15" s="45"/>
-      <c r="U15" s="45"/>
-      <c r="V15" s="45"/>
-      <c r="W15" s="45"/>
-      <c r="X15" s="45"/>
-      <c r="Y15" s="45"/>
-      <c r="Z15" s="44"/>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="P16" s="45"/>
-      <c r="Q16" s="45"/>
-      <c r="R16" s="45"/>
-      <c r="S16" s="45"/>
-      <c r="T16" s="45"/>
-      <c r="U16" s="45"/>
-      <c r="V16" s="45"/>
-      <c r="W16" s="45"/>
-      <c r="X16" s="45"/>
-      <c r="Y16" s="45"/>
-      <c r="Z16" s="44"/>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="P17" s="45"/>
-      <c r="Q17" s="45"/>
-      <c r="R17" s="45"/>
-      <c r="S17" s="45"/>
-      <c r="T17" s="45"/>
-      <c r="U17" s="45"/>
-      <c r="V17" s="45"/>
-      <c r="W17" s="45"/>
-      <c r="X17" s="45"/>
-      <c r="Y17" s="45"/>
-      <c r="Z17" s="44"/>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="P18" s="45"/>
-      <c r="Q18" s="45"/>
-      <c r="R18" s="45"/>
-      <c r="S18" s="45"/>
-      <c r="T18" s="45"/>
-      <c r="U18" s="45"/>
-      <c r="V18" s="45"/>
-      <c r="W18" s="45"/>
-      <c r="X18" s="45"/>
-      <c r="Y18" s="45"/>
-      <c r="Z18" s="44"/>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="P19" s="45"/>
-      <c r="Q19" s="45"/>
-      <c r="R19" s="45"/>
-      <c r="S19" s="45"/>
-      <c r="T19" s="45"/>
-      <c r="U19" s="45"/>
-      <c r="V19" s="45"/>
-      <c r="W19" s="45"/>
-      <c r="X19" s="45"/>
-      <c r="Y19" s="45"/>
-      <c r="Z19" s="44"/>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A20" s="41" t="s">
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A20" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="B20" s="41"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="41"/>
-      <c r="L20" s="41"/>
-      <c r="M20" s="41"/>
-      <c r="N20" s="41"/>
-      <c r="O20" s="41"/>
-      <c r="P20" s="45"/>
-      <c r="Q20" s="45"/>
-      <c r="R20" s="45"/>
-      <c r="S20" s="45"/>
-      <c r="T20" s="45"/>
-      <c r="U20" s="45"/>
-      <c r="V20" s="45"/>
-      <c r="W20" s="45"/>
-      <c r="X20" s="45"/>
-      <c r="Y20" s="45"/>
-      <c r="Z20" s="44"/>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A21" s="42"/>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
-      <c r="P21" s="45"/>
-      <c r="Q21" s="45"/>
-      <c r="R21" s="45"/>
-      <c r="S21" s="45"/>
-      <c r="T21" s="45"/>
-      <c r="U21" s="45"/>
-      <c r="V21" s="45"/>
-      <c r="W21" s="45"/>
-      <c r="X21" s="45"/>
-      <c r="Y21" s="45"/>
-      <c r="Z21" s="44"/>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A22" s="49" t="s">
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="28"/>
+      <c r="L20" s="28"/>
+      <c r="M20" s="28"/>
+      <c r="N20" s="28"/>
+      <c r="O20" s="28"/>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A21" s="29"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+      <c r="K21" s="29"/>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A22" s="31" t="s">
         <v>139</v>
       </c>
-      <c r="B22" s="42"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
-      <c r="P22" s="45"/>
-      <c r="Q22" s="45"/>
-      <c r="R22" s="45"/>
-      <c r="S22" s="45"/>
-      <c r="T22" s="45"/>
-      <c r="U22" s="45"/>
-      <c r="V22" s="45"/>
-      <c r="W22" s="45"/>
-      <c r="X22" s="45"/>
-      <c r="Y22" s="45"/>
-      <c r="Z22" s="44"/>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A23" s="49" t="s">
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="29"/>
+      <c r="F22" s="29"/>
+      <c r="G22" s="29"/>
+      <c r="H22" s="29"/>
+      <c r="I22" s="29"/>
+      <c r="J22" s="29"/>
+      <c r="K22" s="29"/>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="31" t="s">
         <v>140</v>
       </c>
-      <c r="B23" s="42"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
-      <c r="P23" s="45"/>
-      <c r="Q23" s="45"/>
-      <c r="R23" s="45"/>
-      <c r="S23" s="45"/>
-      <c r="T23" s="45"/>
-      <c r="U23" s="45"/>
-      <c r="V23" s="45"/>
-      <c r="W23" s="45"/>
-      <c r="X23" s="45"/>
-      <c r="Y23" s="45"/>
-      <c r="Z23" s="44"/>
-    </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A24" s="49" t="s">
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="29"/>
+      <c r="F23" s="29"/>
+      <c r="G23" s="29"/>
+      <c r="H23" s="29"/>
+      <c r="I23" s="29"/>
+      <c r="J23" s="29"/>
+      <c r="K23" s="29"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
         <v>141</v>
       </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="P24" s="45"/>
-      <c r="Q24" s="45"/>
-      <c r="R24" s="45"/>
-      <c r="S24" s="45"/>
-      <c r="T24" s="45"/>
-      <c r="U24" s="45"/>
-      <c r="V24" s="45"/>
-      <c r="W24" s="45"/>
-      <c r="X24" s="45"/>
-      <c r="Y24" s="45"/>
-      <c r="Z24" s="44"/>
-    </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A25" s="49" t="s">
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="29"/>
+      <c r="F24" s="29"/>
+      <c r="G24" s="29"/>
+      <c r="H24" s="29"/>
+      <c r="I24" s="29"/>
+      <c r="J24" s="29"/>
+      <c r="K24" s="29"/>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A25" s="31" t="s">
         <v>142</v>
       </c>
-      <c r="B25" s="42"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
-      <c r="P25" s="45"/>
-      <c r="Q25" s="45"/>
-      <c r="R25" s="45"/>
-      <c r="S25" s="45"/>
-      <c r="T25" s="45"/>
-      <c r="U25" s="45"/>
-      <c r="V25" s="45"/>
-      <c r="W25" s="45"/>
-      <c r="X25" s="45"/>
-      <c r="Y25" s="45"/>
-      <c r="Z25" s="44"/>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A26" s="42"/>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
-      <c r="P26" s="45"/>
-      <c r="Q26" s="45"/>
-      <c r="R26" s="45"/>
-      <c r="S26" s="45"/>
-      <c r="T26" s="45"/>
-      <c r="U26" s="45"/>
-      <c r="V26" s="45"/>
-      <c r="W26" s="45"/>
-      <c r="X26" s="45"/>
-      <c r="Y26" s="45"/>
-      <c r="Z26" s="44"/>
-    </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A27" s="42"/>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
-      <c r="K27" s="42"/>
-      <c r="P27" s="45"/>
-      <c r="Q27" s="45"/>
-      <c r="R27" s="45"/>
-      <c r="S27" s="45"/>
-      <c r="T27" s="45"/>
-      <c r="U27" s="45"/>
-      <c r="V27" s="45"/>
-      <c r="W27" s="45"/>
-      <c r="X27" s="45"/>
-      <c r="Y27" s="45"/>
-      <c r="Z27" s="44"/>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A28" s="42"/>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
-      <c r="K28" s="42"/>
-      <c r="P28" s="45"/>
-      <c r="Q28" s="45"/>
-      <c r="R28" s="45"/>
-      <c r="S28" s="45"/>
-      <c r="T28" s="45"/>
-      <c r="U28" s="45"/>
-      <c r="V28" s="45"/>
-      <c r="W28" s="45"/>
-      <c r="X28" s="45"/>
-      <c r="Y28" s="45"/>
-      <c r="Z28" s="44"/>
-    </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="P29" s="45"/>
-      <c r="Q29" s="45"/>
-      <c r="R29" s="45"/>
-      <c r="S29" s="45"/>
-      <c r="T29" s="45"/>
-      <c r="U29" s="45"/>
-      <c r="V29" s="45"/>
-      <c r="W29" s="45"/>
-      <c r="X29" s="45"/>
-      <c r="Y29" s="45"/>
-      <c r="Z29" s="44"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="29"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="29"/>
+      <c r="I25" s="29"/>
+      <c r="J25" s="29"/>
+      <c r="K25" s="29"/>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A26" s="31" t="s">
+        <v>143</v>
+      </c>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="29"/>
+      <c r="E26" s="29"/>
+      <c r="F26" s="29"/>
+      <c r="G26" s="29"/>
+      <c r="H26" s="29"/>
+      <c r="I26" s="29"/>
+      <c r="J26" s="29"/>
+      <c r="K26" s="29"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A27" s="29"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="29"/>
+      <c r="E27" s="29"/>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="29"/>
+      <c r="I27" s="29"/>
+      <c r="J27" s="29"/>
+      <c r="K27" s="29"/>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A28" s="29"/>
+      <c r="B28" s="29"/>
+      <c r="C28" s="29"/>
+      <c r="D28" s="29"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="29"/>
+      <c r="G28" s="29"/>
+      <c r="H28" s="29"/>
+      <c r="I28" s="29"/>
+      <c r="J28" s="29"/>
+      <c r="K28" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3140,12 +2853,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" s="8" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="36" t="s">
+      <c r="B2" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
     </row>
     <row r="4" spans="2:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="17" t="s">
@@ -3183,10 +2896,10 @@
       <c r="C8" s="13"/>
     </row>
     <row r="9" spans="2:5" s="14" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="33"/>
+      <c r="C9" s="39"/>
       <c r="D9" s="15" t="s">
         <v>1</v>
       </c>
@@ -3195,184 +2908,184 @@
       </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
+      <c r="C10" s="37"/>
+      <c r="D10" s="37"/>
+      <c r="E10" s="37"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="29"/>
+      <c r="C11" s="35"/>
       <c r="D11" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E11" s="11"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="C12" s="29"/>
+      <c r="C12" s="35"/>
       <c r="D12" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E12" s="11"/>
     </row>
     <row r="13" spans="2:5" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="29"/>
+      <c r="C13" s="35"/>
       <c r="D13" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E13" s="11"/>
     </row>
     <row r="14" spans="2:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="29"/>
+      <c r="C14" s="35"/>
       <c r="D14" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E14" s="11"/>
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="29"/>
+      <c r="C15" s="35"/>
       <c r="D15" s="10" t="s">
         <v>118</v>
       </c>
       <c r="E15" s="11"/>
     </row>
     <row r="16" spans="2:5" ht="51" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="29"/>
+      <c r="C16" s="35"/>
       <c r="D16" s="10" t="s">
         <v>119</v>
       </c>
       <c r="E16" s="11"/>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="37"/>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="35" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="29"/>
+      <c r="C18" s="35"/>
       <c r="D18" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E18" s="11"/>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="29"/>
+      <c r="C19" s="35"/>
       <c r="D19" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E19" s="11"/>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="35" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="29"/>
+      <c r="C20" s="35"/>
       <c r="D20" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E20" s="11"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="29"/>
+      <c r="C21" s="35"/>
       <c r="D21" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E21" s="11"/>
     </row>
     <row r="22" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="C22" s="29"/>
+      <c r="C22" s="35"/>
       <c r="D22" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E22" s="11"/>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="29"/>
+      <c r="C23" s="35"/>
       <c r="D23" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E23" s="11"/>
     </row>
     <row r="24" spans="2:6" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="29"/>
+      <c r="C24" s="35"/>
       <c r="D24" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E24" s="11"/>
     </row>
     <row r="25" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="31" t="s">
+      <c r="B25" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="C25" s="31"/>
+      <c r="C25" s="42"/>
       <c r="D25" s="23" t="s">
         <v>117</v>
       </c>
       <c r="E25" s="24"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="35"/>
+      <c r="C26" s="41"/>
       <c r="D26" s="23"/>
       <c r="E26" s="24"/>
     </row>
     <row r="27" spans="2:6" ht="55.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="31" t="s">
+      <c r="B27" s="42" t="s">
         <v>110</v>
       </c>
-      <c r="C27" s="31"/>
+      <c r="C27" s="42"/>
       <c r="D27" s="23" t="s">
         <v>117</v>
       </c>
       <c r="E27" s="24"/>
     </row>
     <row r="28" spans="2:6" ht="63" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="26" t="s">
+      <c r="B28" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="C28" s="27"/>
+      <c r="C28" s="45"/>
       <c r="D28" s="10" t="s">
         <v>117</v>
       </c>
@@ -3382,10 +3095,10 @@
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B29" s="26" t="s">
+      <c r="B29" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="C29" s="27"/>
+      <c r="C29" s="45"/>
       <c r="D29" s="10" t="s">
         <v>117</v>
       </c>
@@ -3395,128 +3108,128 @@
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B30" s="31" t="s">
+      <c r="B30" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="C30" s="31"/>
+      <c r="C30" s="42"/>
       <c r="D30" s="23" t="s">
         <v>117</v>
       </c>
       <c r="E30" s="24"/>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30"/>
-      <c r="E31" s="30"/>
+      <c r="C31" s="46"/>
+      <c r="D31" s="46"/>
+      <c r="E31" s="46"/>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="31" t="s">
+      <c r="B32" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="31"/>
+      <c r="C32" s="42"/>
       <c r="D32" s="23" t="s">
         <v>117</v>
       </c>
       <c r="E32" s="24"/>
     </row>
     <row r="33" spans="2:6" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="31" t="s">
+      <c r="B33" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C33" s="31"/>
+      <c r="C33" s="42"/>
       <c r="D33" s="23" t="s">
         <v>117</v>
       </c>
       <c r="E33" s="24"/>
     </row>
     <row r="34" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="31" t="s">
+      <c r="B34" s="42" t="s">
         <v>16</v>
       </c>
-      <c r="C34" s="31"/>
+      <c r="C34" s="42"/>
       <c r="D34" s="23" t="s">
         <v>117</v>
       </c>
       <c r="E34" s="24"/>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B35" s="31" t="s">
+      <c r="B35" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="C35" s="31"/>
+      <c r="C35" s="42"/>
       <c r="D35" s="23" t="s">
         <v>118</v>
       </c>
       <c r="E35" s="24"/>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="31" t="s">
+      <c r="B36" s="42" t="s">
         <v>105</v>
       </c>
-      <c r="C36" s="31"/>
+      <c r="C36" s="42"/>
       <c r="D36" s="23" t="s">
         <v>117</v>
       </c>
       <c r="E36" s="24"/>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="31" t="s">
+      <c r="B37" s="42" t="s">
         <v>106</v>
       </c>
-      <c r="C37" s="31"/>
+      <c r="C37" s="42"/>
       <c r="D37" s="23" t="s">
         <v>117</v>
       </c>
       <c r="E37" s="24"/>
     </row>
     <row r="38" spans="2:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="29" t="s">
+      <c r="B38" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="C38" s="29"/>
+      <c r="C38" s="35"/>
       <c r="D38" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E38" s="11"/>
     </row>
     <row r="39" spans="2:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="29" t="s">
+      <c r="B39" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="29"/>
+      <c r="C39" s="35"/>
       <c r="D39" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E39" s="11"/>
     </row>
     <row r="40" spans="2:6" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="29" t="s">
+      <c r="B40" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="C40" s="29"/>
+      <c r="C40" s="35"/>
       <c r="D40" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E40" s="11"/>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="29" t="s">
+      <c r="B41" s="35" t="s">
         <v>58</v>
       </c>
-      <c r="C41" s="29"/>
+      <c r="C41" s="35"/>
       <c r="D41" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E41" s="11"/>
     </row>
     <row r="42" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="28" t="s">
+      <c r="B42" s="43" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="28"/>
+      <c r="C42" s="43"/>
       <c r="D42" s="10" t="s">
         <v>117</v>
       </c>
@@ -3526,170 +3239,170 @@
       </c>
     </row>
     <row r="43" spans="2:6" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="29" t="s">
+      <c r="B43" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="29"/>
+      <c r="C43" s="35"/>
       <c r="D43" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E43" s="11"/>
     </row>
     <row r="44" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="29" t="s">
+      <c r="B44" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="C44" s="29"/>
+      <c r="C44" s="35"/>
       <c r="D44" s="10" t="s">
         <v>119</v>
       </c>
       <c r="E44" s="11"/>
     </row>
     <row r="45" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="29" t="s">
+      <c r="B45" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="29"/>
+      <c r="C45" s="35"/>
       <c r="D45" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E45" s="11"/>
     </row>
     <row r="46" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="29" t="s">
+      <c r="B46" s="35" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="29"/>
+      <c r="C46" s="35"/>
       <c r="D46" s="10" t="s">
         <v>118</v>
       </c>
       <c r="E46" s="11"/>
     </row>
     <row r="47" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="29" t="s">
+      <c r="B47" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="29"/>
+      <c r="C47" s="35"/>
       <c r="D47" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E47" s="11"/>
     </row>
     <row r="48" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="29" t="s">
+      <c r="B48" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="C48" s="29"/>
+      <c r="C48" s="35"/>
       <c r="D48" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E48" s="11"/>
     </row>
     <row r="49" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B49" s="29" t="s">
+      <c r="B49" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="C49" s="29"/>
+      <c r="C49" s="35"/>
       <c r="D49" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E49" s="11"/>
     </row>
     <row r="50" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B50" s="29" t="s">
+      <c r="B50" s="35" t="s">
         <v>68</v>
       </c>
-      <c r="C50" s="29"/>
+      <c r="C50" s="35"/>
       <c r="D50" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E50" s="11"/>
     </row>
     <row r="51" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B51" s="29" t="s">
+      <c r="B51" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="C51" s="29"/>
+      <c r="C51" s="35"/>
       <c r="D51" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E51" s="11"/>
     </row>
     <row r="52" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="29" t="s">
+      <c r="B52" s="35" t="s">
         <v>69</v>
       </c>
-      <c r="C52" s="29"/>
+      <c r="C52" s="35"/>
       <c r="D52" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E52" s="11"/>
     </row>
     <row r="53" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B53" s="29" t="s">
+      <c r="B53" s="35" t="s">
         <v>70</v>
       </c>
-      <c r="C53" s="29"/>
+      <c r="C53" s="35"/>
       <c r="D53" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E53" s="11"/>
     </row>
     <row r="54" spans="2:6" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B54" s="28" t="s">
+      <c r="B54" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="C54" s="28"/>
+      <c r="C54" s="43"/>
       <c r="D54" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E54" s="11"/>
     </row>
     <row r="55" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="29" t="s">
+      <c r="B55" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="C55" s="29"/>
+      <c r="C55" s="35"/>
       <c r="D55" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E55" s="11"/>
     </row>
     <row r="56" spans="2:6" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="28" t="s">
+      <c r="B56" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="C56" s="28"/>
+      <c r="C56" s="43"/>
       <c r="D56" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E56" s="11"/>
     </row>
     <row r="57" spans="2:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B57" s="28" t="s">
+      <c r="B57" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="C57" s="28"/>
+      <c r="C57" s="43"/>
       <c r="D57" s="10" t="s">
         <v>119</v>
       </c>
       <c r="E57" s="11"/>
     </row>
     <row r="58" spans="2:6" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B58" s="28" t="s">
+      <c r="B58" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="C58" s="28"/>
+      <c r="C58" s="43"/>
       <c r="D58" s="10" t="s">
         <v>117</v>
       </c>
       <c r="E58" s="11"/>
     </row>
     <row r="59" spans="2:6" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="28" t="s">
+      <c r="B59" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="C59" s="28"/>
+      <c r="C59" s="43"/>
       <c r="D59" s="10" t="s">
         <v>117</v>
       </c>
@@ -3760,6 +3473,42 @@
     </row>
   </sheetData>
   <mergeCells count="52">
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B50:C50"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B31:E31"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B32:C32"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B12:C12"/>
     <mergeCell ref="B13:C13"/>
@@ -3776,42 +3525,6 @@
     <mergeCell ref="B22:C22"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B9:C9"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B46:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="B54:C54"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B31:E31"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B42:C42"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B45:C45"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D65547:D65584 IU65547:IU65584 SQ65547:SQ65584 ACM65547:ACM65584 AMI65547:AMI65584 AWE65547:AWE65584 BGA65547:BGA65584 BPW65547:BPW65584 BZS65547:BZS65584 CJO65547:CJO65584 CTK65547:CTK65584 DDG65547:DDG65584 DNC65547:DNC65584 DWY65547:DWY65584 EGU65547:EGU65584 EQQ65547:EQQ65584 FAM65547:FAM65584 FKI65547:FKI65584 FUE65547:FUE65584 GEA65547:GEA65584 GNW65547:GNW65584 GXS65547:GXS65584 HHO65547:HHO65584 HRK65547:HRK65584 IBG65547:IBG65584 ILC65547:ILC65584 IUY65547:IUY65584 JEU65547:JEU65584 JOQ65547:JOQ65584 JYM65547:JYM65584 KII65547:KII65584 KSE65547:KSE65584 LCA65547:LCA65584 LLW65547:LLW65584 LVS65547:LVS65584 MFO65547:MFO65584 MPK65547:MPK65584 MZG65547:MZG65584 NJC65547:NJC65584 NSY65547:NSY65584 OCU65547:OCU65584 OMQ65547:OMQ65584 OWM65547:OWM65584 PGI65547:PGI65584 PQE65547:PQE65584 QAA65547:QAA65584 QJW65547:QJW65584 QTS65547:QTS65584 RDO65547:RDO65584 RNK65547:RNK65584 RXG65547:RXG65584 SHC65547:SHC65584 SQY65547:SQY65584 TAU65547:TAU65584 TKQ65547:TKQ65584 TUM65547:TUM65584 UEI65547:UEI65584 UOE65547:UOE65584 UYA65547:UYA65584 VHW65547:VHW65584 VRS65547:VRS65584 WBO65547:WBO65584 WLK65547:WLK65584 WVG65547:WVG65584 D131083:D131120 IU131083:IU131120 SQ131083:SQ131120 ACM131083:ACM131120 AMI131083:AMI131120 AWE131083:AWE131120 BGA131083:BGA131120 BPW131083:BPW131120 BZS131083:BZS131120 CJO131083:CJO131120 CTK131083:CTK131120 DDG131083:DDG131120 DNC131083:DNC131120 DWY131083:DWY131120 EGU131083:EGU131120 EQQ131083:EQQ131120 FAM131083:FAM131120 FKI131083:FKI131120 FUE131083:FUE131120 GEA131083:GEA131120 GNW131083:GNW131120 GXS131083:GXS131120 HHO131083:HHO131120 HRK131083:HRK131120 IBG131083:IBG131120 ILC131083:ILC131120 IUY131083:IUY131120 JEU131083:JEU131120 JOQ131083:JOQ131120 JYM131083:JYM131120 KII131083:KII131120 KSE131083:KSE131120 LCA131083:LCA131120 LLW131083:LLW131120 LVS131083:LVS131120 MFO131083:MFO131120 MPK131083:MPK131120 MZG131083:MZG131120 NJC131083:NJC131120 NSY131083:NSY131120 OCU131083:OCU131120 OMQ131083:OMQ131120 OWM131083:OWM131120 PGI131083:PGI131120 PQE131083:PQE131120 QAA131083:QAA131120 QJW131083:QJW131120 QTS131083:QTS131120 RDO131083:RDO131120 RNK131083:RNK131120 RXG131083:RXG131120 SHC131083:SHC131120 SQY131083:SQY131120 TAU131083:TAU131120 TKQ131083:TKQ131120 TUM131083:TUM131120 UEI131083:UEI131120 UOE131083:UOE131120 UYA131083:UYA131120 VHW131083:VHW131120 VRS131083:VRS131120 WBO131083:WBO131120 WLK131083:WLK131120 WVG131083:WVG131120 D196619:D196656 IU196619:IU196656 SQ196619:SQ196656 ACM196619:ACM196656 AMI196619:AMI196656 AWE196619:AWE196656 BGA196619:BGA196656 BPW196619:BPW196656 BZS196619:BZS196656 CJO196619:CJO196656 CTK196619:CTK196656 DDG196619:DDG196656 DNC196619:DNC196656 DWY196619:DWY196656 EGU196619:EGU196656 EQQ196619:EQQ196656 FAM196619:FAM196656 FKI196619:FKI196656 FUE196619:FUE196656 GEA196619:GEA196656 GNW196619:GNW196656 GXS196619:GXS196656 HHO196619:HHO196656 HRK196619:HRK196656 IBG196619:IBG196656 ILC196619:ILC196656 IUY196619:IUY196656 JEU196619:JEU196656 JOQ196619:JOQ196656 JYM196619:JYM196656 KII196619:KII196656 KSE196619:KSE196656 LCA196619:LCA196656 LLW196619:LLW196656 LVS196619:LVS196656 MFO196619:MFO196656 MPK196619:MPK196656 MZG196619:MZG196656 NJC196619:NJC196656 NSY196619:NSY196656 OCU196619:OCU196656 OMQ196619:OMQ196656 OWM196619:OWM196656 PGI196619:PGI196656 PQE196619:PQE196656 QAA196619:QAA196656 QJW196619:QJW196656 QTS196619:QTS196656 RDO196619:RDO196656 RNK196619:RNK196656 RXG196619:RXG196656 SHC196619:SHC196656 SQY196619:SQY196656 TAU196619:TAU196656 TKQ196619:TKQ196656 TUM196619:TUM196656 UEI196619:UEI196656 UOE196619:UOE196656 UYA196619:UYA196656 VHW196619:VHW196656 VRS196619:VRS196656 WBO196619:WBO196656 WLK196619:WLK196656 WVG196619:WVG196656 D262155:D262192 IU262155:IU262192 SQ262155:SQ262192 ACM262155:ACM262192 AMI262155:AMI262192 AWE262155:AWE262192 BGA262155:BGA262192 BPW262155:BPW262192 BZS262155:BZS262192 CJO262155:CJO262192 CTK262155:CTK262192 DDG262155:DDG262192 DNC262155:DNC262192 DWY262155:DWY262192 EGU262155:EGU262192 EQQ262155:EQQ262192 FAM262155:FAM262192 FKI262155:FKI262192 FUE262155:FUE262192 GEA262155:GEA262192 GNW262155:GNW262192 GXS262155:GXS262192 HHO262155:HHO262192 HRK262155:HRK262192 IBG262155:IBG262192 ILC262155:ILC262192 IUY262155:IUY262192 JEU262155:JEU262192 JOQ262155:JOQ262192 JYM262155:JYM262192 KII262155:KII262192 KSE262155:KSE262192 LCA262155:LCA262192 LLW262155:LLW262192 LVS262155:LVS262192 MFO262155:MFO262192 MPK262155:MPK262192 MZG262155:MZG262192 NJC262155:NJC262192 NSY262155:NSY262192 OCU262155:OCU262192 OMQ262155:OMQ262192 OWM262155:OWM262192 PGI262155:PGI262192 PQE262155:PQE262192 QAA262155:QAA262192 QJW262155:QJW262192 QTS262155:QTS262192 RDO262155:RDO262192 RNK262155:RNK262192 RXG262155:RXG262192 SHC262155:SHC262192 SQY262155:SQY262192 TAU262155:TAU262192 TKQ262155:TKQ262192 TUM262155:TUM262192 UEI262155:UEI262192 UOE262155:UOE262192 UYA262155:UYA262192 VHW262155:VHW262192 VRS262155:VRS262192 WBO262155:WBO262192 WLK262155:WLK262192 WVG262155:WVG262192 D327691:D327728 IU327691:IU327728 SQ327691:SQ327728 ACM327691:ACM327728 AMI327691:AMI327728 AWE327691:AWE327728 BGA327691:BGA327728 BPW327691:BPW327728 BZS327691:BZS327728 CJO327691:CJO327728 CTK327691:CTK327728 DDG327691:DDG327728 DNC327691:DNC327728 DWY327691:DWY327728 EGU327691:EGU327728 EQQ327691:EQQ327728 FAM327691:FAM327728 FKI327691:FKI327728 FUE327691:FUE327728 GEA327691:GEA327728 GNW327691:GNW327728 GXS327691:GXS327728 HHO327691:HHO327728 HRK327691:HRK327728 IBG327691:IBG327728 ILC327691:ILC327728 IUY327691:IUY327728 JEU327691:JEU327728 JOQ327691:JOQ327728 JYM327691:JYM327728 KII327691:KII327728 KSE327691:KSE327728 LCA327691:LCA327728 LLW327691:LLW327728 LVS327691:LVS327728 MFO327691:MFO327728 MPK327691:MPK327728 MZG327691:MZG327728 NJC327691:NJC327728 NSY327691:NSY327728 OCU327691:OCU327728 OMQ327691:OMQ327728 OWM327691:OWM327728 PGI327691:PGI327728 PQE327691:PQE327728 QAA327691:QAA327728 QJW327691:QJW327728 QTS327691:QTS327728 RDO327691:RDO327728 RNK327691:RNK327728 RXG327691:RXG327728 SHC327691:SHC327728 SQY327691:SQY327728 TAU327691:TAU327728 TKQ327691:TKQ327728 TUM327691:TUM327728 UEI327691:UEI327728 UOE327691:UOE327728 UYA327691:UYA327728 VHW327691:VHW327728 VRS327691:VRS327728 WBO327691:WBO327728 WLK327691:WLK327728 WVG327691:WVG327728 D393227:D393264 IU393227:IU393264 SQ393227:SQ393264 ACM393227:ACM393264 AMI393227:AMI393264 AWE393227:AWE393264 BGA393227:BGA393264 BPW393227:BPW393264 BZS393227:BZS393264 CJO393227:CJO393264 CTK393227:CTK393264 DDG393227:DDG393264 DNC393227:DNC393264 DWY393227:DWY393264 EGU393227:EGU393264 EQQ393227:EQQ393264 FAM393227:FAM393264 FKI393227:FKI393264 FUE393227:FUE393264 GEA393227:GEA393264 GNW393227:GNW393264 GXS393227:GXS393264 HHO393227:HHO393264 HRK393227:HRK393264 IBG393227:IBG393264 ILC393227:ILC393264 IUY393227:IUY393264 JEU393227:JEU393264 JOQ393227:JOQ393264 JYM393227:JYM393264 KII393227:KII393264 KSE393227:KSE393264 LCA393227:LCA393264 LLW393227:LLW393264 LVS393227:LVS393264 MFO393227:MFO393264 MPK393227:MPK393264 MZG393227:MZG393264 NJC393227:NJC393264 NSY393227:NSY393264 OCU393227:OCU393264 OMQ393227:OMQ393264 OWM393227:OWM393264 PGI393227:PGI393264 PQE393227:PQE393264 QAA393227:QAA393264 QJW393227:QJW393264 QTS393227:QTS393264 RDO393227:RDO393264 RNK393227:RNK393264 RXG393227:RXG393264 SHC393227:SHC393264 SQY393227:SQY393264 TAU393227:TAU393264 TKQ393227:TKQ393264 TUM393227:TUM393264 UEI393227:UEI393264 UOE393227:UOE393264 UYA393227:UYA393264 VHW393227:VHW393264 VRS393227:VRS393264 WBO393227:WBO393264 WLK393227:WLK393264 WVG393227:WVG393264 D458763:D458800 IU458763:IU458800 SQ458763:SQ458800 ACM458763:ACM458800 AMI458763:AMI458800 AWE458763:AWE458800 BGA458763:BGA458800 BPW458763:BPW458800 BZS458763:BZS458800 CJO458763:CJO458800 CTK458763:CTK458800 DDG458763:DDG458800 DNC458763:DNC458800 DWY458763:DWY458800 EGU458763:EGU458800 EQQ458763:EQQ458800 FAM458763:FAM458800 FKI458763:FKI458800 FUE458763:FUE458800 GEA458763:GEA458800 GNW458763:GNW458800 GXS458763:GXS458800 HHO458763:HHO458800 HRK458763:HRK458800 IBG458763:IBG458800 ILC458763:ILC458800 IUY458763:IUY458800 JEU458763:JEU458800 JOQ458763:JOQ458800 JYM458763:JYM458800 KII458763:KII458800 KSE458763:KSE458800 LCA458763:LCA458800 LLW458763:LLW458800 LVS458763:LVS458800 MFO458763:MFO458800 MPK458763:MPK458800 MZG458763:MZG458800 NJC458763:NJC458800 NSY458763:NSY458800 OCU458763:OCU458800 OMQ458763:OMQ458800 OWM458763:OWM458800 PGI458763:PGI458800 PQE458763:PQE458800 QAA458763:QAA458800 QJW458763:QJW458800 QTS458763:QTS458800 RDO458763:RDO458800 RNK458763:RNK458800 RXG458763:RXG458800 SHC458763:SHC458800 SQY458763:SQY458800 TAU458763:TAU458800 TKQ458763:TKQ458800 TUM458763:TUM458800 UEI458763:UEI458800 UOE458763:UOE458800 UYA458763:UYA458800 VHW458763:VHW458800 VRS458763:VRS458800 WBO458763:WBO458800 WLK458763:WLK458800 WVG458763:WVG458800 D524299:D524336 IU524299:IU524336 SQ524299:SQ524336 ACM524299:ACM524336 AMI524299:AMI524336 AWE524299:AWE524336 BGA524299:BGA524336 BPW524299:BPW524336 BZS524299:BZS524336 CJO524299:CJO524336 CTK524299:CTK524336 DDG524299:DDG524336 DNC524299:DNC524336 DWY524299:DWY524336 EGU524299:EGU524336 EQQ524299:EQQ524336 FAM524299:FAM524336 FKI524299:FKI524336 FUE524299:FUE524336 GEA524299:GEA524336 GNW524299:GNW524336 GXS524299:GXS524336 HHO524299:HHO524336 HRK524299:HRK524336 IBG524299:IBG524336 ILC524299:ILC524336 IUY524299:IUY524336 JEU524299:JEU524336 JOQ524299:JOQ524336 JYM524299:JYM524336 KII524299:KII524336 KSE524299:KSE524336 LCA524299:LCA524336 LLW524299:LLW524336 LVS524299:LVS524336 MFO524299:MFO524336 MPK524299:MPK524336 MZG524299:MZG524336 NJC524299:NJC524336 NSY524299:NSY524336 OCU524299:OCU524336 OMQ524299:OMQ524336 OWM524299:OWM524336 PGI524299:PGI524336 PQE524299:PQE524336 QAA524299:QAA524336 QJW524299:QJW524336 QTS524299:QTS524336 RDO524299:RDO524336 RNK524299:RNK524336 RXG524299:RXG524336 SHC524299:SHC524336 SQY524299:SQY524336 TAU524299:TAU524336 TKQ524299:TKQ524336 TUM524299:TUM524336 UEI524299:UEI524336 UOE524299:UOE524336 UYA524299:UYA524336 VHW524299:VHW524336 VRS524299:VRS524336 WBO524299:WBO524336 WLK524299:WLK524336 WVG524299:WVG524336 D589835:D589872 IU589835:IU589872 SQ589835:SQ589872 ACM589835:ACM589872 AMI589835:AMI589872 AWE589835:AWE589872 BGA589835:BGA589872 BPW589835:BPW589872 BZS589835:BZS589872 CJO589835:CJO589872 CTK589835:CTK589872 DDG589835:DDG589872 DNC589835:DNC589872 DWY589835:DWY589872 EGU589835:EGU589872 EQQ589835:EQQ589872 FAM589835:FAM589872 FKI589835:FKI589872 FUE589835:FUE589872 GEA589835:GEA589872 GNW589835:GNW589872 GXS589835:GXS589872 HHO589835:HHO589872 HRK589835:HRK589872 IBG589835:IBG589872 ILC589835:ILC589872 IUY589835:IUY589872 JEU589835:JEU589872 JOQ589835:JOQ589872 JYM589835:JYM589872 KII589835:KII589872 KSE589835:KSE589872 LCA589835:LCA589872 LLW589835:LLW589872 LVS589835:LVS589872 MFO589835:MFO589872 MPK589835:MPK589872 MZG589835:MZG589872 NJC589835:NJC589872 NSY589835:NSY589872 OCU589835:OCU589872 OMQ589835:OMQ589872 OWM589835:OWM589872 PGI589835:PGI589872 PQE589835:PQE589872 QAA589835:QAA589872 QJW589835:QJW589872 QTS589835:QTS589872 RDO589835:RDO589872 RNK589835:RNK589872 RXG589835:RXG589872 SHC589835:SHC589872 SQY589835:SQY589872 TAU589835:TAU589872 TKQ589835:TKQ589872 TUM589835:TUM589872 UEI589835:UEI589872 UOE589835:UOE589872 UYA589835:UYA589872 VHW589835:VHW589872 VRS589835:VRS589872 WBO589835:WBO589872 WLK589835:WLK589872 WVG589835:WVG589872 D655371:D655408 IU655371:IU655408 SQ655371:SQ655408 ACM655371:ACM655408 AMI655371:AMI655408 AWE655371:AWE655408 BGA655371:BGA655408 BPW655371:BPW655408 BZS655371:BZS655408 CJO655371:CJO655408 CTK655371:CTK655408 DDG655371:DDG655408 DNC655371:DNC655408 DWY655371:DWY655408 EGU655371:EGU655408 EQQ655371:EQQ655408 FAM655371:FAM655408 FKI655371:FKI655408 FUE655371:FUE655408 GEA655371:GEA655408 GNW655371:GNW655408 GXS655371:GXS655408 HHO655371:HHO655408 HRK655371:HRK655408 IBG655371:IBG655408 ILC655371:ILC655408 IUY655371:IUY655408 JEU655371:JEU655408 JOQ655371:JOQ655408 JYM655371:JYM655408 KII655371:KII655408 KSE655371:KSE655408 LCA655371:LCA655408 LLW655371:LLW655408 LVS655371:LVS655408 MFO655371:MFO655408 MPK655371:MPK655408 MZG655371:MZG655408 NJC655371:NJC655408 NSY655371:NSY655408 OCU655371:OCU655408 OMQ655371:OMQ655408 OWM655371:OWM655408 PGI655371:PGI655408 PQE655371:PQE655408 QAA655371:QAA655408 QJW655371:QJW655408 QTS655371:QTS655408 RDO655371:RDO655408 RNK655371:RNK655408 RXG655371:RXG655408 SHC655371:SHC655408 SQY655371:SQY655408 TAU655371:TAU655408 TKQ655371:TKQ655408 TUM655371:TUM655408 UEI655371:UEI655408 UOE655371:UOE655408 UYA655371:UYA655408 VHW655371:VHW655408 VRS655371:VRS655408 WBO655371:WBO655408 WLK655371:WLK655408 WVG655371:WVG655408 D720907:D720944 IU720907:IU720944 SQ720907:SQ720944 ACM720907:ACM720944 AMI720907:AMI720944 AWE720907:AWE720944 BGA720907:BGA720944 BPW720907:BPW720944 BZS720907:BZS720944 CJO720907:CJO720944 CTK720907:CTK720944 DDG720907:DDG720944 DNC720907:DNC720944 DWY720907:DWY720944 EGU720907:EGU720944 EQQ720907:EQQ720944 FAM720907:FAM720944 FKI720907:FKI720944 FUE720907:FUE720944 GEA720907:GEA720944 GNW720907:GNW720944 GXS720907:GXS720944 HHO720907:HHO720944 HRK720907:HRK720944 IBG720907:IBG720944 ILC720907:ILC720944 IUY720907:IUY720944 JEU720907:JEU720944 JOQ720907:JOQ720944 JYM720907:JYM720944 KII720907:KII720944 KSE720907:KSE720944 LCA720907:LCA720944 LLW720907:LLW720944 LVS720907:LVS720944 MFO720907:MFO720944 MPK720907:MPK720944 MZG720907:MZG720944 NJC720907:NJC720944 NSY720907:NSY720944 OCU720907:OCU720944 OMQ720907:OMQ720944 OWM720907:OWM720944 PGI720907:PGI720944 PQE720907:PQE720944 QAA720907:QAA720944 QJW720907:QJW720944 QTS720907:QTS720944 RDO720907:RDO720944 RNK720907:RNK720944 RXG720907:RXG720944 SHC720907:SHC720944 SQY720907:SQY720944 TAU720907:TAU720944 TKQ720907:TKQ720944 TUM720907:TUM720944 UEI720907:UEI720944 UOE720907:UOE720944 UYA720907:UYA720944 VHW720907:VHW720944 VRS720907:VRS720944 WBO720907:WBO720944 WLK720907:WLK720944 WVG720907:WVG720944 D786443:D786480 IU786443:IU786480 SQ786443:SQ786480 ACM786443:ACM786480 AMI786443:AMI786480 AWE786443:AWE786480 BGA786443:BGA786480 BPW786443:BPW786480 BZS786443:BZS786480 CJO786443:CJO786480 CTK786443:CTK786480 DDG786443:DDG786480 DNC786443:DNC786480 DWY786443:DWY786480 EGU786443:EGU786480 EQQ786443:EQQ786480 FAM786443:FAM786480 FKI786443:FKI786480 FUE786443:FUE786480 GEA786443:GEA786480 GNW786443:GNW786480 GXS786443:GXS786480 HHO786443:HHO786480 HRK786443:HRK786480 IBG786443:IBG786480 ILC786443:ILC786480 IUY786443:IUY786480 JEU786443:JEU786480 JOQ786443:JOQ786480 JYM786443:JYM786480 KII786443:KII786480 KSE786443:KSE786480 LCA786443:LCA786480 LLW786443:LLW786480 LVS786443:LVS786480 MFO786443:MFO786480 MPK786443:MPK786480 MZG786443:MZG786480 NJC786443:NJC786480 NSY786443:NSY786480 OCU786443:OCU786480 OMQ786443:OMQ786480 OWM786443:OWM786480 PGI786443:PGI786480 PQE786443:PQE786480 QAA786443:QAA786480 QJW786443:QJW786480 QTS786443:QTS786480 RDO786443:RDO786480 RNK786443:RNK786480 RXG786443:RXG786480 SHC786443:SHC786480 SQY786443:SQY786480 TAU786443:TAU786480 TKQ786443:TKQ786480 TUM786443:TUM786480 UEI786443:UEI786480 UOE786443:UOE786480 UYA786443:UYA786480 VHW786443:VHW786480 VRS786443:VRS786480 WBO786443:WBO786480 WLK786443:WLK786480 WVG786443:WVG786480 D851979:D852016 IU851979:IU852016 SQ851979:SQ852016 ACM851979:ACM852016 AMI851979:AMI852016 AWE851979:AWE852016 BGA851979:BGA852016 BPW851979:BPW852016 BZS851979:BZS852016 CJO851979:CJO852016 CTK851979:CTK852016 DDG851979:DDG852016 DNC851979:DNC852016 DWY851979:DWY852016 EGU851979:EGU852016 EQQ851979:EQQ852016 FAM851979:FAM852016 FKI851979:FKI852016 FUE851979:FUE852016 GEA851979:GEA852016 GNW851979:GNW852016 GXS851979:GXS852016 HHO851979:HHO852016 HRK851979:HRK852016 IBG851979:IBG852016 ILC851979:ILC852016 IUY851979:IUY852016 JEU851979:JEU852016 JOQ851979:JOQ852016 JYM851979:JYM852016 KII851979:KII852016 KSE851979:KSE852016 LCA851979:LCA852016 LLW851979:LLW852016 LVS851979:LVS852016 MFO851979:MFO852016 MPK851979:MPK852016 MZG851979:MZG852016 NJC851979:NJC852016 NSY851979:NSY852016 OCU851979:OCU852016 OMQ851979:OMQ852016 OWM851979:OWM852016 PGI851979:PGI852016 PQE851979:PQE852016 QAA851979:QAA852016 QJW851979:QJW852016 QTS851979:QTS852016 RDO851979:RDO852016 RNK851979:RNK852016 RXG851979:RXG852016 SHC851979:SHC852016 SQY851979:SQY852016 TAU851979:TAU852016 TKQ851979:TKQ852016 TUM851979:TUM852016 UEI851979:UEI852016 UOE851979:UOE852016 UYA851979:UYA852016 VHW851979:VHW852016 VRS851979:VRS852016 WBO851979:WBO852016 WLK851979:WLK852016 WVG851979:WVG852016 D917515:D917552 IU917515:IU917552 SQ917515:SQ917552 ACM917515:ACM917552 AMI917515:AMI917552 AWE917515:AWE917552 BGA917515:BGA917552 BPW917515:BPW917552 BZS917515:BZS917552 CJO917515:CJO917552 CTK917515:CTK917552 DDG917515:DDG917552 DNC917515:DNC917552 DWY917515:DWY917552 EGU917515:EGU917552 EQQ917515:EQQ917552 FAM917515:FAM917552 FKI917515:FKI917552 FUE917515:FUE917552 GEA917515:GEA917552 GNW917515:GNW917552 GXS917515:GXS917552 HHO917515:HHO917552 HRK917515:HRK917552 IBG917515:IBG917552 ILC917515:ILC917552 IUY917515:IUY917552 JEU917515:JEU917552 JOQ917515:JOQ917552 JYM917515:JYM917552 KII917515:KII917552 KSE917515:KSE917552 LCA917515:LCA917552 LLW917515:LLW917552 LVS917515:LVS917552 MFO917515:MFO917552 MPK917515:MPK917552 MZG917515:MZG917552 NJC917515:NJC917552 NSY917515:NSY917552 OCU917515:OCU917552 OMQ917515:OMQ917552 OWM917515:OWM917552 PGI917515:PGI917552 PQE917515:PQE917552 QAA917515:QAA917552 QJW917515:QJW917552 QTS917515:QTS917552 RDO917515:RDO917552 RNK917515:RNK917552 RXG917515:RXG917552 SHC917515:SHC917552 SQY917515:SQY917552 TAU917515:TAU917552 TKQ917515:TKQ917552 TUM917515:TUM917552 UEI917515:UEI917552 UOE917515:UOE917552 UYA917515:UYA917552 VHW917515:VHW917552 VRS917515:VRS917552 WBO917515:WBO917552 WLK917515:WLK917552 WVG917515:WVG917552 D983051:D983088 IU983051:IU983088 SQ983051:SQ983088 ACM983051:ACM983088 AMI983051:AMI983088 AWE983051:AWE983088 BGA983051:BGA983088 BPW983051:BPW983088 BZS983051:BZS983088 CJO983051:CJO983088 CTK983051:CTK983088 DDG983051:DDG983088 DNC983051:DNC983088 DWY983051:DWY983088 EGU983051:EGU983088 EQQ983051:EQQ983088 FAM983051:FAM983088 FKI983051:FKI983088 FUE983051:FUE983088 GEA983051:GEA983088 GNW983051:GNW983088 GXS983051:GXS983088 HHO983051:HHO983088 HRK983051:HRK983088 IBG983051:IBG983088 ILC983051:ILC983088 IUY983051:IUY983088 JEU983051:JEU983088 JOQ983051:JOQ983088 JYM983051:JYM983088 KII983051:KII983088 KSE983051:KSE983088 LCA983051:LCA983088 LLW983051:LLW983088 LVS983051:LVS983088 MFO983051:MFO983088 MPK983051:MPK983088 MZG983051:MZG983088 NJC983051:NJC983088 NSY983051:NSY983088 OCU983051:OCU983088 OMQ983051:OMQ983088 OWM983051:OWM983088 PGI983051:PGI983088 PQE983051:PQE983088 QAA983051:QAA983088 QJW983051:QJW983088 QTS983051:QTS983088 RDO983051:RDO983088 RNK983051:RNK983088 RXG983051:RXG983088 SHC983051:SHC983088 SQY983051:SQY983088 TAU983051:TAU983088 TKQ983051:TKQ983088 TUM983051:TUM983088 UEI983051:UEI983088 UOE983051:UOE983088 UYA983051:UYA983088 VHW983051:VHW983088 VRS983051:VRS983088 WBO983051:WBO983088 WLK983051:WLK983088 WVG983051:WVG983088 D11:D16 D18:D59 WBO11:WBO59 VRS11:VRS59 VHW11:VHW59 UYA11:UYA59 UOE11:UOE59 UEI11:UEI59 TUM11:TUM59 TKQ11:TKQ59 TAU11:TAU59 SQY11:SQY59 SHC11:SHC59 RXG11:RXG59 RNK11:RNK59 RDO11:RDO59 QTS11:QTS59 QJW11:QJW59 QAA11:QAA59 PQE11:PQE59 PGI11:PGI59 OWM11:OWM59 OMQ11:OMQ59 OCU11:OCU59 NSY11:NSY59 NJC11:NJC59 MZG11:MZG59 MPK11:MPK59 MFO11:MFO59 LVS11:LVS59 LLW11:LLW59 LCA11:LCA59 KSE11:KSE59 KII11:KII59 JYM11:JYM59 JOQ11:JOQ59 JEU11:JEU59 IUY11:IUY59 ILC11:ILC59 IBG11:IBG59 HRK11:HRK59 HHO11:HHO59 GXS11:GXS59 GNW11:GNW59 GEA11:GEA59 FUE11:FUE59 FKI11:FKI59 FAM11:FAM59 EQQ11:EQQ59 EGU11:EGU59 DWY11:DWY59 DNC11:DNC59 DDG11:DDG59 CTK11:CTK59 CJO11:CJO59 BZS11:BZS59 BPW11:BPW59 BGA11:BGA59 AWE11:AWE59 AMI11:AMI59 ACM11:ACM59 SQ11:SQ59 IU11:IU59 WLK11:WLK59 WVG11:WVG59" xr:uid="{00000000-0002-0000-0200-000000000000}">

</xml_diff>